<commit_message>
cleaned treatment, added scapring csv with new data and worked on USDA
</commit_message>
<xml_diff>
--- a/analyses/scrapeUSDAseedmanual/scraping/usdaDataScraping_CRD.xlsx
+++ b/analyses/scrapeUSDAseedmanual/scraping/usdaDataScraping_CRD.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christophe_rouleau-desrochers/github/egret/analyses/scrapeUSDAseedmanual/scraping/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCC5544C-43E8-EE4C-BF6E-9A271C705DB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1867F29B-ADA1-0B4D-ACB0-E1BD7483F99A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29400" yWindow="-2480" windowWidth="38400" windowHeight="21600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Meta" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="215">
   <si>
     <t>pdf_page_number</t>
   </si>
@@ -438,18 +438,9 @@
     <t>5</t>
   </si>
   <si>
-    <t>25 and 5</t>
-  </si>
-  <si>
-    <t>20 and 4</t>
-  </si>
-  <si>
     <t>4.5</t>
   </si>
   <si>
-    <t>18.5 and 4.5</t>
-  </si>
-  <si>
     <t>20 and 3</t>
   </si>
   <si>
@@ -703,6 +694,18 @@
   </si>
   <si>
     <t>47 to 61</t>
+  </si>
+  <si>
+    <t>warm_stratification_days2</t>
+  </si>
+  <si>
+    <t>warm_stratification_temp_C</t>
+  </si>
+  <si>
+    <t>cold_stratification_temp_C</t>
+  </si>
+  <si>
+    <t>25</t>
   </si>
 </sst>
 </file>
@@ -765,7 +768,13 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="32">
+  <dxfs count="34">
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
@@ -876,45 +885,41 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9970B36A-C938-554F-9718-360E80C161BA}" name="Table2" displayName="Table2" ref="A1:AD47" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
-  <autoFilter ref="A1:AD47" xr:uid="{9970B36A-C938-554F-9718-360E80C161BA}">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="magnolia"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
-  <tableColumns count="30">
-    <tableColumn id="1" xr3:uid="{B704D3DD-BCF1-2048-BE97-C249C1BDB66E}" name="pdf_page_number" dataDxfId="29"/>
-    <tableColumn id="2" xr3:uid="{3E94C656-E5E6-3E4B-8DA6-85820D32A6BF}" name="pdf_table_number" dataDxfId="28"/>
-    <tableColumn id="3" xr3:uid="{4996521F-8EC2-2A40-9174-2F8614329D42}" name="genus_name" dataDxfId="27"/>
-    <tableColumn id="4" xr3:uid="{80F9C112-39B8-DE44-8471-099B486B5F4A}" name="species_name" dataDxfId="26"/>
-    <tableColumn id="5" xr3:uid="{375B4BEA-646E-5446-894A-9B9469DB02A7}" name="seed_source" dataDxfId="25"/>
-    <tableColumn id="6" xr3:uid="{72890B4B-A941-274D-90C5-B0090D70148A}" name="medium" dataDxfId="24"/>
-    <tableColumn id="7" xr3:uid="{7657C123-FA50-ED46-A76A-26AE17978143}" name="pregermination_treatment_time_minutes" dataDxfId="23"/>
-    <tableColumn id="8" xr3:uid="{25D42B2B-7F05-4140-A3C6-F8B396550CAB}" name="pregermination_treatment_hot_water_soak_C" dataDxfId="22"/>
-    <tableColumn id="9" xr3:uid="{55A4F340-7B6D-7943-8B39-CFAE9E6FE33F}" name="pretreatment" dataDxfId="21"/>
-    <tableColumn id="10" xr3:uid="{4A6EEDC6-97D1-5C4D-8AA2-6F5DFBF4D1C4}" name="stratification_temp_C" dataDxfId="20"/>
-    <tableColumn id="11" xr3:uid="{DEEF428E-8BC4-ED4F-A0A2-906B50FA71DD}" name="warm_stratification_days" dataDxfId="19"/>
-    <tableColumn id="12" xr3:uid="{93B28E55-01FC-F64C-9809-1780CA274A58}" name="cold_stratification_days" dataDxfId="18"/>
-    <tableColumn id="13" xr3:uid="{FBA71BC1-6F33-B742-9505-31E5F69BC022}" name="dailyl_light_hours" dataDxfId="17"/>
-    <tableColumn id="14" xr3:uid="{B60543C3-E2EE-A64E-A396-1C242453800C}" name="day_temp_celsius" dataDxfId="16"/>
-    <tableColumn id="15" xr3:uid="{A98F0563-6BD3-C049-89CC-CCFA69D88415}" name="night_temp_celsius" dataDxfId="15"/>
-    <tableColumn id="16" xr3:uid="{441701F9-64D9-6C4C-98DD-50E953D9AE81}" name="temp_unspecified_time_of_day_celsius" dataDxfId="14"/>
-    <tableColumn id="17" xr3:uid="{8E32E59C-2511-5E47-B942-01EF1C2F823C}" name="test_duration_in_days" dataDxfId="13"/>
-    <tableColumn id="18" xr3:uid="{427BB247-5A32-DE42-AC51-6837CDABE181}" name="germination_time_days" dataDxfId="12"/>
-    <tableColumn id="19" xr3:uid="{35DE5AFC-901F-3445-96DA-507E967B4ECB}" name="total_germination_percent" dataDxfId="11"/>
-    <tableColumn id="20" xr3:uid="{BC769C61-E4F8-114A-B837-872ED1FFEAAC}" name="avg_germination_percent" dataDxfId="10"/>
-    <tableColumn id="21" xr3:uid="{093E7249-8AC3-8044-8840-C1350D4C13FA}" name="samples" dataDxfId="9"/>
-    <tableColumn id="22" xr3:uid="{4AAA545E-A06B-5A49-A9C2-811A91D56309}" name="germination_rate" dataDxfId="8"/>
-    <tableColumn id="23" xr3:uid="{0E3380FC-04AB-B648-BA64-33C0172712E8}" name="avg_germinative_energy_percent" dataDxfId="7"/>
-    <tableColumn id="24" xr3:uid="{BB029E85-4EEF-7541-A8A6-B78FC45AA990}" name="germinative_energy_percent" dataDxfId="6"/>
-    <tableColumn id="25" xr3:uid="{D9A90743-B6FB-BA4B-951F-4B5A9FC761BA}" name="avg_germinative_capacity" dataDxfId="5"/>
-    <tableColumn id="26" xr3:uid="{5AE4612B-E138-4D40-8419-CC14A92B62CD}" name="germinative_capacity" dataDxfId="4"/>
-    <tableColumn id="27" xr3:uid="{5BE09F3B-7D66-884A-B192-CEE49F2B845E}" name="percent_germination_15degC_incubated" dataDxfId="3"/>
-    <tableColumn id="28" xr3:uid="{6061511F-2CE6-FF4C-BA21-079020EC6884}" name="percent_germination_20degC_incubated" dataDxfId="2"/>
-    <tableColumn id="29" xr3:uid="{B17A6158-E57A-8B49-B7C6-A792A8BB3857}" name="50%_germ" dataDxfId="1"/>
-    <tableColumn id="30" xr3:uid="{C6852079-746D-E843-96F0-451DDB3F34C3}" name="Notes" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9970B36A-C938-554F-9718-360E80C161BA}" name="Table2" displayName="Table2" ref="A1:AF47" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
+  <autoFilter ref="A1:AF47" xr:uid="{9970B36A-C938-554F-9718-360E80C161BA}"/>
+  <tableColumns count="32">
+    <tableColumn id="1" xr3:uid="{B704D3DD-BCF1-2048-BE97-C249C1BDB66E}" name="pdf_page_number" dataDxfId="31"/>
+    <tableColumn id="2" xr3:uid="{3E94C656-E5E6-3E4B-8DA6-85820D32A6BF}" name="pdf_table_number" dataDxfId="30"/>
+    <tableColumn id="3" xr3:uid="{4996521F-8EC2-2A40-9174-2F8614329D42}" name="genus_name" dataDxfId="29"/>
+    <tableColumn id="4" xr3:uid="{80F9C112-39B8-DE44-8471-099B486B5F4A}" name="species_name" dataDxfId="28"/>
+    <tableColumn id="5" xr3:uid="{375B4BEA-646E-5446-894A-9B9469DB02A7}" name="seed_source" dataDxfId="27"/>
+    <tableColumn id="6" xr3:uid="{72890B4B-A941-274D-90C5-B0090D70148A}" name="medium" dataDxfId="26"/>
+    <tableColumn id="7" xr3:uid="{7657C123-FA50-ED46-A76A-26AE17978143}" name="pregermination_treatment_time_minutes" dataDxfId="25"/>
+    <tableColumn id="8" xr3:uid="{25D42B2B-7F05-4140-A3C6-F8B396550CAB}" name="pregermination_treatment_hot_water_soak_C" dataDxfId="24"/>
+    <tableColumn id="9" xr3:uid="{55A4F340-7B6D-7943-8B39-CFAE9E6FE33F}" name="pretreatment" dataDxfId="23"/>
+    <tableColumn id="10" xr3:uid="{4A6EEDC6-97D1-5C4D-8AA2-6F5DFBF4D1C4}" name="stratification_temp_C" dataDxfId="22"/>
+    <tableColumn id="31" xr3:uid="{C2EB3AFD-A023-9943-99AC-88FDB5F21DAA}" name="warm_stratification_temp_C" dataDxfId="1"/>
+    <tableColumn id="32" xr3:uid="{722DB568-4A1B-2143-82BA-AA33796FD61E}" name="cold_stratification_temp_C" dataDxfId="0"/>
+    <tableColumn id="11" xr3:uid="{DEEF428E-8BC4-ED4F-A0A2-906B50FA71DD}" name="warm_stratification_days2" dataDxfId="21"/>
+    <tableColumn id="12" xr3:uid="{93B28E55-01FC-F64C-9809-1780CA274A58}" name="cold_stratification_days" dataDxfId="20"/>
+    <tableColumn id="13" xr3:uid="{FBA71BC1-6F33-B742-9505-31E5F69BC022}" name="dailyl_light_hours" dataDxfId="19"/>
+    <tableColumn id="14" xr3:uid="{B60543C3-E2EE-A64E-A396-1C242453800C}" name="day_temp_celsius" dataDxfId="18"/>
+    <tableColumn id="15" xr3:uid="{A98F0563-6BD3-C049-89CC-CCFA69D88415}" name="night_temp_celsius" dataDxfId="17"/>
+    <tableColumn id="16" xr3:uid="{441701F9-64D9-6C4C-98DD-50E953D9AE81}" name="temp_unspecified_time_of_day_celsius" dataDxfId="16"/>
+    <tableColumn id="17" xr3:uid="{8E32E59C-2511-5E47-B942-01EF1C2F823C}" name="test_duration_in_days" dataDxfId="15"/>
+    <tableColumn id="18" xr3:uid="{427BB247-5A32-DE42-AC51-6837CDABE181}" name="germination_time_days" dataDxfId="14"/>
+    <tableColumn id="19" xr3:uid="{35DE5AFC-901F-3445-96DA-507E967B4ECB}" name="total_germination_percent" dataDxfId="13"/>
+    <tableColumn id="20" xr3:uid="{BC769C61-E4F8-114A-B837-872ED1FFEAAC}" name="avg_germination_percent" dataDxfId="12"/>
+    <tableColumn id="21" xr3:uid="{093E7249-8AC3-8044-8840-C1350D4C13FA}" name="samples" dataDxfId="11"/>
+    <tableColumn id="22" xr3:uid="{4AAA545E-A06B-5A49-A9C2-811A91D56309}" name="germination_rate" dataDxfId="10"/>
+    <tableColumn id="23" xr3:uid="{0E3380FC-04AB-B648-BA64-33C0172712E8}" name="avg_germinative_energy_percent" dataDxfId="9"/>
+    <tableColumn id="24" xr3:uid="{BB029E85-4EEF-7541-A8A6-B78FC45AA990}" name="germinative_energy_percent" dataDxfId="8"/>
+    <tableColumn id="25" xr3:uid="{D9A90743-B6FB-BA4B-951F-4B5A9FC761BA}" name="avg_germinative_capacity" dataDxfId="7"/>
+    <tableColumn id="26" xr3:uid="{5AE4612B-E138-4D40-8419-CC14A92B62CD}" name="germinative_capacity" dataDxfId="6"/>
+    <tableColumn id="27" xr3:uid="{5BE09F3B-7D66-884A-B192-CEE49F2B845E}" name="percent_germination_15degC_incubated" dataDxfId="5"/>
+    <tableColumn id="28" xr3:uid="{6061511F-2CE6-FF4C-BA21-079020EC6884}" name="percent_germination_20degC_incubated" dataDxfId="4"/>
+    <tableColumn id="29" xr3:uid="{B17A6158-E57A-8B49-B7C6-A792A8BB3857}" name="50%_germ" dataDxfId="3"/>
+    <tableColumn id="30" xr3:uid="{C6852079-746D-E843-96F0-451DDB3F34C3}" name="Notes" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1506,10 +1511,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4AC4DDB-17EE-463A-9304-F699F6DBC2E2}">
-  <dimension ref="A1:AD47"/>
+  <dimension ref="A1:AF47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X1" zoomScale="187" workbookViewId="0">
-      <selection activeCell="Z2" sqref="Z2"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="187" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1523,28 +1528,29 @@
     <col min="8" max="8" width="37.1640625" customWidth="1"/>
     <col min="9" max="9" width="12" customWidth="1"/>
     <col min="10" max="10" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.5" customWidth="1"/>
-    <col min="14" max="14" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="34.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="20.83203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="22" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="25" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="30" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="26.5" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="36.1640625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="20.5" customWidth="1"/>
+    <col min="13" max="13" width="23" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.5" customWidth="1"/>
+    <col min="16" max="16" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="34.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="22" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="25" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="30" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="26.5" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="29" max="30" width="36.1640625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="8.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1576,67 +1582,73 @@
         <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>10</v>
+        <v>212</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AE1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>703</v>
       </c>
@@ -1660,41 +1672,43 @@
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
-      <c r="N2" s="3" t="s">
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="Q2" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="P2" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q2" s="3"/>
       <c r="R2" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="S2" s="3" t="s">
-        <v>76</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="S2" s="3"/>
       <c r="T2" s="3" t="s">
-        <v>76</v>
+        <v>207</v>
       </c>
       <c r="U2" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="W2" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="V2" s="3"/>
-      <c r="W2" s="3"/>
       <c r="X2" s="3"/>
-      <c r="Y2" s="3" t="s">
-        <v>206</v>
-      </c>
+      <c r="Y2" s="3"/>
       <c r="Z2" s="3"/>
-      <c r="AA2" s="3"/>
+      <c r="AA2" s="3" t="s">
+        <v>203</v>
+      </c>
       <c r="AB2" s="3"/>
       <c r="AC2" s="3"/>
       <c r="AD2" s="3"/>
-    </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AE2" s="3"/>
+      <c r="AF2" s="3"/>
+    </row>
+    <row r="3" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>703</v>
       </c>
@@ -1718,41 +1732,43 @@
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
-      <c r="N3" s="3">
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3">
         <v>30</v>
       </c>
-      <c r="O3" s="3">
+      <c r="Q3" s="3">
         <v>20</v>
       </c>
-      <c r="P3" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q3" s="3"/>
       <c r="R3" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="S3" s="3" t="s">
-        <v>76</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="S3" s="3"/>
       <c r="T3" s="3" t="s">
-        <v>76</v>
+        <v>208</v>
       </c>
       <c r="U3" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="V3" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="W3" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="V3" s="3"/>
-      <c r="W3" s="3"/>
       <c r="X3" s="3"/>
-      <c r="Y3" s="3" t="s">
-        <v>207</v>
-      </c>
+      <c r="Y3" s="3"/>
       <c r="Z3" s="3"/>
-      <c r="AA3" s="3"/>
+      <c r="AA3" s="3" t="s">
+        <v>204</v>
+      </c>
       <c r="AB3" s="3"/>
       <c r="AC3" s="3"/>
       <c r="AD3" s="3"/>
-    </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AE3" s="3"/>
+      <c r="AF3" s="3"/>
+    </row>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>703</v>
       </c>
@@ -1776,41 +1792,43 @@
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
-      <c r="N4" s="3">
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3">
         <v>30</v>
       </c>
-      <c r="O4" s="3">
+      <c r="Q4" s="3">
         <v>20</v>
       </c>
-      <c r="P4" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q4" s="3"/>
       <c r="R4" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="S4" s="3" t="s">
-        <v>76</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="S4" s="3"/>
       <c r="T4" s="3" t="s">
-        <v>76</v>
+        <v>209</v>
       </c>
       <c r="U4" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="V4" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="W4" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="V4" s="3"/>
-      <c r="W4" s="3"/>
       <c r="X4" s="3"/>
-      <c r="Y4" s="3" t="s">
-        <v>208</v>
-      </c>
+      <c r="Y4" s="3"/>
       <c r="Z4" s="3"/>
-      <c r="AA4" s="3"/>
+      <c r="AA4" s="3" t="s">
+        <v>205</v>
+      </c>
       <c r="AB4" s="3"/>
       <c r="AC4" s="3"/>
       <c r="AD4" s="3"/>
-    </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AE4" s="3"/>
+      <c r="AF4" s="3"/>
+    </row>
+    <row r="5" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>703</v>
       </c>
@@ -1834,41 +1852,43 @@
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
       <c r="M5" s="3"/>
-      <c r="N5" s="3">
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3">
         <v>22</v>
       </c>
-      <c r="O5" s="3">
+      <c r="Q5" s="3">
         <v>22</v>
       </c>
-      <c r="P5" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q5" s="3"/>
-      <c r="R5" s="3">
+      <c r="R5" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="S5" s="3"/>
+      <c r="T5" s="3">
         <v>35</v>
       </c>
-      <c r="S5" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="T5" s="3" t="s">
-        <v>76</v>
-      </c>
       <c r="U5" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="V5" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="W5" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="V5" s="3"/>
-      <c r="W5" s="3"/>
       <c r="X5" s="3"/>
-      <c r="Y5" s="3" t="s">
+      <c r="Y5" s="3"/>
+      <c r="Z5" s="3"/>
+      <c r="AA5" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="Z5" s="3"/>
-      <c r="AA5" s="3"/>
       <c r="AB5" s="3"/>
       <c r="AC5" s="3"/>
       <c r="AD5" s="3"/>
-    </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AE5" s="3"/>
+      <c r="AF5" s="3"/>
+    </row>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>703</v>
       </c>
@@ -1892,41 +1912,43 @@
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
-      <c r="N6" s="3">
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3">
         <v>24</v>
       </c>
-      <c r="O6" s="3">
+      <c r="Q6" s="3">
         <v>30</v>
       </c>
-      <c r="P6" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q6" s="3"/>
-      <c r="R6" s="3">
+      <c r="R6" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="S6" s="3"/>
+      <c r="T6" s="3">
         <v>44</v>
       </c>
-      <c r="S6" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="T6" s="3" t="s">
-        <v>76</v>
-      </c>
       <c r="U6" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="V6" s="3"/>
-      <c r="W6" s="3"/>
+      <c r="V6" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="W6" s="3" t="s">
+        <v>76</v>
+      </c>
       <c r="X6" s="3"/>
-      <c r="Y6" s="3" t="s">
+      <c r="Y6" s="3"/>
+      <c r="Z6" s="3"/>
+      <c r="AA6" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="Z6" s="3"/>
-      <c r="AA6" s="3"/>
       <c r="AB6" s="3"/>
       <c r="AC6" s="3"/>
       <c r="AD6" s="3"/>
-    </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AE6" s="3"/>
+      <c r="AF6" s="3"/>
+    </row>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>703</v>
       </c>
@@ -1952,45 +1974,47 @@
         <v>76</v>
       </c>
       <c r="K7" s="3"/>
-      <c r="L7" s="3" t="s">
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="M7" s="3"/>
-      <c r="N7" s="3">
+      <c r="O7" s="3"/>
+      <c r="P7" s="3">
         <v>18</v>
       </c>
-      <c r="O7" s="3">
+      <c r="Q7" s="3">
         <v>18</v>
       </c>
-      <c r="P7" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q7" s="3"/>
-      <c r="R7" s="3">
+      <c r="R7" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="S7" s="3"/>
+      <c r="T7" s="3">
         <v>33</v>
       </c>
-      <c r="S7" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="T7" s="3" t="s">
-        <v>76</v>
-      </c>
       <c r="U7" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="V7" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="W7" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="V7" s="3"/>
-      <c r="W7" s="3"/>
       <c r="X7" s="3"/>
-      <c r="Y7" s="3" t="s">
+      <c r="Y7" s="3"/>
+      <c r="Z7" s="3"/>
+      <c r="AA7" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="Z7" s="3"/>
-      <c r="AA7" s="3"/>
       <c r="AB7" s="3"/>
       <c r="AC7" s="3"/>
       <c r="AD7" s="3"/>
-    </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AE7" s="3"/>
+      <c r="AF7" s="3"/>
+    </row>
+    <row r="8" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>703</v>
       </c>
@@ -2014,41 +2038,43 @@
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
-      <c r="N8" s="3">
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3">
         <v>30</v>
       </c>
-      <c r="O8" s="3">
+      <c r="Q8" s="3">
         <v>20</v>
       </c>
-      <c r="P8" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q8" s="3"/>
       <c r="R8" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="S8" s="3" t="s">
-        <v>76</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="S8" s="3"/>
       <c r="T8" s="3" t="s">
-        <v>76</v>
+        <v>210</v>
       </c>
       <c r="U8" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="V8" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="W8" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="V8" s="3"/>
-      <c r="W8" s="3"/>
       <c r="X8" s="3"/>
-      <c r="Y8" s="3" t="s">
-        <v>209</v>
-      </c>
+      <c r="Y8" s="3"/>
       <c r="Z8" s="3"/>
-      <c r="AA8" s="3"/>
+      <c r="AA8" s="3" t="s">
+        <v>206</v>
+      </c>
       <c r="AB8" s="3"/>
       <c r="AC8" s="3"/>
       <c r="AD8" s="3"/>
-    </row>
-    <row r="9" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AE8" s="3"/>
+      <c r="AF8" s="3"/>
+    </row>
+    <row r="9" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>105</v>
       </c>
@@ -2066,30 +2092,30 @@
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
       <c r="I9" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="J9" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="K9" s="3" t="s">
+      <c r="M9" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="L9" s="3" t="s">
+      <c r="N9" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="M9" s="3"/>
-      <c r="N9" s="3"/>
       <c r="O9" s="3"/>
-      <c r="P9" s="3" t="s">
+      <c r="P9" s="3"/>
+      <c r="Q9" s="3"/>
+      <c r="R9" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="Q9" s="3"/>
-      <c r="R9" s="3"/>
-      <c r="S9" s="3" t="s">
+      <c r="S9" s="3"/>
+      <c r="T9" s="3"/>
+      <c r="U9" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="T9" s="3"/>
-      <c r="U9" s="3"/>
       <c r="V9" s="3"/>
       <c r="W9" s="3"/>
       <c r="X9" s="3"/>
@@ -2098,11 +2124,13 @@
       <c r="AA9" s="3"/>
       <c r="AB9" s="3"/>
       <c r="AC9" s="3"/>
-      <c r="AD9" s="3" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="10" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AD9" s="3"/>
+      <c r="AE9" s="3"/>
+      <c r="AF9" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="10" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>105</v>
       </c>
@@ -2120,30 +2148,32 @@
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
       <c r="I10" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="J10" s="3" t="s">
-        <v>125</v>
-      </c>
+        <v>152</v>
+      </c>
+      <c r="J10" s="3"/>
       <c r="K10" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="M10" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="L10" s="3" t="s">
+      <c r="N10" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="M10" s="3"/>
-      <c r="N10" s="3"/>
       <c r="O10" s="3"/>
-      <c r="P10" s="4" t="s">
-        <v>149</v>
-      </c>
+      <c r="P10" s="3"/>
       <c r="Q10" s="3"/>
-      <c r="R10" s="3"/>
-      <c r="S10" s="3" t="s">
+      <c r="R10" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="S10" s="3"/>
+      <c r="T10" s="3"/>
+      <c r="U10" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="T10" s="3"/>
-      <c r="U10" s="3"/>
       <c r="V10" s="3"/>
       <c r="W10" s="3"/>
       <c r="X10" s="3"/>
@@ -2152,11 +2182,13 @@
       <c r="AA10" s="3"/>
       <c r="AB10" s="3"/>
       <c r="AC10" s="3"/>
-      <c r="AD10" s="3" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="11" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AD10" s="3"/>
+      <c r="AE10" s="3"/>
+      <c r="AF10" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="11" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>105</v>
       </c>
@@ -2174,30 +2206,30 @@
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
       <c r="I11" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="J11" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="K11" s="3" t="s">
+      <c r="M11" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="L11" s="3" t="s">
+      <c r="N11" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="M11" s="3"/>
-      <c r="N11" s="3"/>
       <c r="O11" s="3"/>
-      <c r="P11" s="3" t="s">
-        <v>150</v>
-      </c>
+      <c r="P11" s="3"/>
       <c r="Q11" s="3"/>
-      <c r="R11" s="3"/>
-      <c r="S11" s="3" t="s">
-        <v>131</v>
-      </c>
+      <c r="R11" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="S11" s="3"/>
       <c r="T11" s="3"/>
-      <c r="U11" s="3"/>
+      <c r="U11" s="3" t="s">
+        <v>128</v>
+      </c>
       <c r="V11" s="3"/>
       <c r="W11" s="3"/>
       <c r="X11" s="3"/>
@@ -2206,11 +2238,13 @@
       <c r="AA11" s="3"/>
       <c r="AB11" s="3"/>
       <c r="AC11" s="3"/>
-      <c r="AD11" s="3" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="12" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AD11" s="3"/>
+      <c r="AE11" s="3"/>
+      <c r="AF11" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="12" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>105</v>
       </c>
@@ -2228,30 +2262,30 @@
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
       <c r="I12" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="J12" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="K12" s="3" t="s">
+      <c r="M12" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="L12" s="3" t="s">
+      <c r="N12" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="M12" s="3"/>
-      <c r="N12" s="3"/>
       <c r="O12" s="3"/>
-      <c r="P12" s="3" t="s">
-        <v>150</v>
-      </c>
+      <c r="P12" s="3"/>
       <c r="Q12" s="3"/>
-      <c r="R12" s="3"/>
-      <c r="S12" s="3" t="s">
-        <v>132</v>
-      </c>
+      <c r="R12" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="S12" s="3"/>
       <c r="T12" s="3"/>
-      <c r="U12" s="3"/>
+      <c r="U12" s="3" t="s">
+        <v>129</v>
+      </c>
       <c r="V12" s="3"/>
       <c r="W12" s="3"/>
       <c r="X12" s="3"/>
@@ -2260,11 +2294,13 @@
       <c r="AA12" s="3"/>
       <c r="AB12" s="3"/>
       <c r="AC12" s="3"/>
-      <c r="AD12" s="3" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="13" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AD12" s="3"/>
+      <c r="AE12" s="3"/>
+      <c r="AF12" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="13" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>105</v>
       </c>
@@ -2282,30 +2318,30 @@
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
       <c r="I13" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="J13" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="K13" s="3" t="s">
+      <c r="M13" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="L13" s="3" t="s">
+      <c r="N13" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="M13" s="3"/>
-      <c r="N13" s="3"/>
       <c r="O13" s="3"/>
-      <c r="P13" s="3" t="s">
-        <v>76</v>
-      </c>
+      <c r="P13" s="3"/>
       <c r="Q13" s="3"/>
-      <c r="R13" s="3"/>
-      <c r="S13" s="3" t="s">
-        <v>133</v>
-      </c>
+      <c r="R13" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="S13" s="3"/>
       <c r="T13" s="3"/>
-      <c r="U13" s="3"/>
+      <c r="U13" s="3" t="s">
+        <v>130</v>
+      </c>
       <c r="V13" s="3"/>
       <c r="W13" s="3"/>
       <c r="X13" s="3"/>
@@ -2315,8 +2351,10 @@
       <c r="AB13" s="3"/>
       <c r="AC13" s="3"/>
       <c r="AD13" s="3"/>
-    </row>
-    <row r="14" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AE13" s="3"/>
+      <c r="AF13" s="3"/>
+    </row>
+    <row r="14" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>105</v>
       </c>
@@ -2334,30 +2372,32 @@
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
       <c r="I14" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="J14" s="3" t="s">
-        <v>126</v>
-      </c>
+        <v>152</v>
+      </c>
+      <c r="J14" s="3"/>
       <c r="K14" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="L14" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="M14" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="L14" s="3" t="s">
+      <c r="N14" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="M14" s="3"/>
-      <c r="N14" s="3"/>
       <c r="O14" s="3"/>
-      <c r="P14" s="3" t="s">
-        <v>76</v>
-      </c>
+      <c r="P14" s="3"/>
       <c r="Q14" s="3"/>
-      <c r="R14" s="3"/>
-      <c r="S14" s="3" t="s">
-        <v>134</v>
-      </c>
+      <c r="R14" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="S14" s="3"/>
       <c r="T14" s="3"/>
-      <c r="U14" s="3"/>
+      <c r="U14" s="3" t="s">
+        <v>131</v>
+      </c>
       <c r="V14" s="3"/>
       <c r="W14" s="3"/>
       <c r="X14" s="3"/>
@@ -2367,8 +2407,10 @@
       <c r="AB14" s="3"/>
       <c r="AC14" s="3"/>
       <c r="AD14" s="3"/>
-    </row>
-    <row r="15" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AE14" s="3"/>
+      <c r="AF14" s="3"/>
+    </row>
+    <row r="15" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>105</v>
       </c>
@@ -2386,30 +2428,32 @@
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
       <c r="I15" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="J15" s="3" t="s">
-        <v>126</v>
-      </c>
+        <v>152</v>
+      </c>
+      <c r="J15" s="3"/>
       <c r="K15" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="L15" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="M15" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="L15" s="3" t="s">
+      <c r="N15" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="M15" s="3"/>
-      <c r="N15" s="3"/>
       <c r="O15" s="3"/>
-      <c r="P15" s="3" t="s">
-        <v>76</v>
-      </c>
+      <c r="P15" s="3"/>
       <c r="Q15" s="3"/>
-      <c r="R15" s="3"/>
-      <c r="S15" s="3" t="s">
-        <v>135</v>
-      </c>
+      <c r="R15" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="S15" s="3"/>
       <c r="T15" s="3"/>
-      <c r="U15" s="3"/>
+      <c r="U15" s="3" t="s">
+        <v>132</v>
+      </c>
       <c r="V15" s="3"/>
       <c r="W15" s="3"/>
       <c r="X15" s="3"/>
@@ -2419,8 +2463,10 @@
       <c r="AB15" s="3"/>
       <c r="AC15" s="3"/>
       <c r="AD15" s="3"/>
-    </row>
-    <row r="16" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AE15" s="3"/>
+      <c r="AF15" s="3"/>
+    </row>
+    <row r="16" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>105</v>
       </c>
@@ -2438,30 +2484,30 @@
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
       <c r="I16" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="J16" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="K16" s="3" t="s">
+      <c r="M16" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="L16" s="3" t="s">
+      <c r="N16" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="M16" s="3"/>
-      <c r="N16" s="3"/>
       <c r="O16" s="3"/>
-      <c r="P16" s="3" t="s">
+      <c r="P16" s="3"/>
+      <c r="Q16" s="3"/>
+      <c r="R16" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="Q16" s="3"/>
-      <c r="R16" s="3"/>
-      <c r="S16" s="3" t="s">
-        <v>136</v>
-      </c>
+      <c r="S16" s="3"/>
       <c r="T16" s="3"/>
-      <c r="U16" s="3"/>
+      <c r="U16" s="3" t="s">
+        <v>133</v>
+      </c>
       <c r="V16" s="3"/>
       <c r="W16" s="3"/>
       <c r="X16" s="3"/>
@@ -2471,8 +2517,10 @@
       <c r="AB16" s="3"/>
       <c r="AC16" s="3"/>
       <c r="AD16" s="3"/>
-    </row>
-    <row r="17" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AE16" s="3"/>
+      <c r="AF16" s="3"/>
+    </row>
+    <row r="17" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>105</v>
       </c>
@@ -2490,30 +2538,30 @@
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
       <c r="I17" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="J17" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="K17" s="3" t="s">
+      <c r="M17" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="L17" s="3" t="s">
+      <c r="N17" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="M17" s="3"/>
-      <c r="N17" s="3"/>
       <c r="O17" s="3"/>
-      <c r="P17" s="3" t="s">
+      <c r="P17" s="3"/>
+      <c r="Q17" s="3"/>
+      <c r="R17" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="Q17" s="3"/>
-      <c r="R17" s="3"/>
-      <c r="S17" s="3" t="s">
-        <v>137</v>
-      </c>
+      <c r="S17" s="3"/>
       <c r="T17" s="3"/>
-      <c r="U17" s="3"/>
+      <c r="U17" s="3" t="s">
+        <v>134</v>
+      </c>
       <c r="V17" s="3"/>
       <c r="W17" s="3"/>
       <c r="X17" s="3"/>
@@ -2523,8 +2571,10 @@
       <c r="AB17" s="3"/>
       <c r="AC17" s="3"/>
       <c r="AD17" s="3"/>
-    </row>
-    <row r="18" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AE17" s="3"/>
+      <c r="AF17" s="3"/>
+    </row>
+    <row r="18" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>105</v>
       </c>
@@ -2542,30 +2592,30 @@
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
       <c r="I18" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="J18" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="K18" s="3" t="s">
+      <c r="M18" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="L18" s="3" t="s">
+      <c r="N18" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="M18" s="3"/>
-      <c r="N18" s="3"/>
       <c r="O18" s="3"/>
-      <c r="P18" s="3" t="s">
-        <v>76</v>
-      </c>
+      <c r="P18" s="3"/>
       <c r="Q18" s="3"/>
-      <c r="R18" s="3"/>
-      <c r="S18" s="3" t="s">
-        <v>138</v>
-      </c>
+      <c r="R18" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="S18" s="3"/>
       <c r="T18" s="3"/>
-      <c r="U18" s="3"/>
+      <c r="U18" s="3" t="s">
+        <v>135</v>
+      </c>
       <c r="V18" s="3"/>
       <c r="W18" s="3"/>
       <c r="X18" s="3"/>
@@ -2575,8 +2625,10 @@
       <c r="AB18" s="3"/>
       <c r="AC18" s="3"/>
       <c r="AD18" s="3"/>
-    </row>
-    <row r="19" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AE18" s="3"/>
+      <c r="AF18" s="3"/>
+    </row>
+    <row r="19" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>105</v>
       </c>
@@ -2594,30 +2646,30 @@
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
       <c r="I19" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="J19" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="K19" s="3" t="s">
+      <c r="M19" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="L19" s="3" t="s">
+      <c r="N19" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="M19" s="3"/>
-      <c r="N19" s="3"/>
       <c r="O19" s="3"/>
-      <c r="P19" s="3" t="s">
-        <v>151</v>
-      </c>
+      <c r="P19" s="3"/>
       <c r="Q19" s="3"/>
-      <c r="R19" s="3"/>
-      <c r="S19" s="3" t="s">
+      <c r="R19" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="S19" s="3"/>
+      <c r="T19" s="3"/>
+      <c r="U19" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="T19" s="3"/>
-      <c r="U19" s="3"/>
       <c r="V19" s="3"/>
       <c r="W19" s="3"/>
       <c r="X19" s="3"/>
@@ -2627,8 +2679,10 @@
       <c r="AB19" s="3"/>
       <c r="AC19" s="3"/>
       <c r="AD19" s="3"/>
-    </row>
-    <row r="20" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AE19" s="3"/>
+      <c r="AF19" s="3"/>
+    </row>
+    <row r="20" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>105</v>
       </c>
@@ -2646,30 +2700,30 @@
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
       <c r="I20" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="J20" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="K20" s="3" t="s">
+      <c r="M20" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="L20" s="3" t="s">
+      <c r="N20" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="M20" s="3"/>
-      <c r="N20" s="3"/>
       <c r="O20" s="3"/>
-      <c r="P20" s="3" t="s">
-        <v>151</v>
-      </c>
+      <c r="P20" s="3"/>
       <c r="Q20" s="3"/>
-      <c r="R20" s="3"/>
-      <c r="S20" s="3" t="s">
+      <c r="R20" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="S20" s="3"/>
+      <c r="T20" s="3"/>
+      <c r="U20" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="T20" s="3"/>
-      <c r="U20" s="3"/>
       <c r="V20" s="3"/>
       <c r="W20" s="3"/>
       <c r="X20" s="3"/>
@@ -2679,8 +2733,10 @@
       <c r="AB20" s="3"/>
       <c r="AC20" s="3"/>
       <c r="AD20" s="3"/>
-    </row>
-    <row r="21" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AE20" s="3"/>
+      <c r="AF20" s="3"/>
+    </row>
+    <row r="21" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>105</v>
       </c>
@@ -2698,30 +2754,30 @@
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
       <c r="I21" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="J21" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="K21" s="3" t="s">
+      <c r="M21" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="L21" s="3" t="s">
+      <c r="N21" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="M21" s="3"/>
-      <c r="N21" s="3"/>
       <c r="O21" s="3"/>
-      <c r="P21" s="3" t="s">
+      <c r="P21" s="3"/>
+      <c r="Q21" s="3"/>
+      <c r="R21" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="Q21" s="3"/>
-      <c r="R21" s="3"/>
-      <c r="S21" s="3" t="s">
-        <v>139</v>
-      </c>
+      <c r="S21" s="3"/>
       <c r="T21" s="3"/>
-      <c r="U21" s="3"/>
+      <c r="U21" s="3" t="s">
+        <v>136</v>
+      </c>
       <c r="V21" s="3"/>
       <c r="W21" s="3"/>
       <c r="X21" s="3"/>
@@ -2731,8 +2787,10 @@
       <c r="AB21" s="3"/>
       <c r="AC21" s="3"/>
       <c r="AD21" s="3"/>
-    </row>
-    <row r="22" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AE21" s="3"/>
+      <c r="AF21" s="3"/>
+    </row>
+    <row r="22" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>105</v>
       </c>
@@ -2750,30 +2808,30 @@
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
       <c r="I22" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="J22" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="K22" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="M22" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="L22" s="3" t="s">
+      <c r="N22" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="M22" s="3"/>
-      <c r="N22" s="3"/>
       <c r="O22" s="3"/>
-      <c r="P22" s="3" t="s">
-        <v>127</v>
-      </c>
+      <c r="P22" s="3"/>
       <c r="Q22" s="3"/>
-      <c r="R22" s="3"/>
-      <c r="S22" s="3" t="s">
-        <v>140</v>
-      </c>
+      <c r="R22" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="S22" s="3"/>
       <c r="T22" s="3"/>
-      <c r="U22" s="3"/>
+      <c r="U22" s="3" t="s">
+        <v>137</v>
+      </c>
       <c r="V22" s="3"/>
       <c r="W22" s="3"/>
       <c r="X22" s="3"/>
@@ -2783,8 +2841,10 @@
       <c r="AB22" s="3"/>
       <c r="AC22" s="3"/>
       <c r="AD22" s="3"/>
-    </row>
-    <row r="23" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AE22" s="3"/>
+      <c r="AF22" s="3"/>
+    </row>
+    <row r="23" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>105</v>
       </c>
@@ -2802,30 +2862,30 @@
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
       <c r="I23" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="J23" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="K23" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="M23" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="L23" s="3" t="s">
+      <c r="N23" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="M23" s="3"/>
-      <c r="N23" s="3"/>
       <c r="O23" s="3"/>
-      <c r="P23" s="3" t="s">
+      <c r="P23" s="3"/>
+      <c r="Q23" s="3"/>
+      <c r="R23" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="Q23" s="3"/>
-      <c r="R23" s="3"/>
-      <c r="S23" s="3" t="s">
-        <v>141</v>
-      </c>
+      <c r="S23" s="3"/>
       <c r="T23" s="3"/>
-      <c r="U23" s="3"/>
+      <c r="U23" s="3" t="s">
+        <v>138</v>
+      </c>
       <c r="V23" s="3"/>
       <c r="W23" s="3"/>
       <c r="X23" s="3"/>
@@ -2835,8 +2895,10 @@
       <c r="AB23" s="3"/>
       <c r="AC23" s="3"/>
       <c r="AD23" s="3"/>
-    </row>
-    <row r="24" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AE23" s="3"/>
+      <c r="AF23" s="3"/>
+    </row>
+    <row r="24" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>105</v>
       </c>
@@ -2854,30 +2916,32 @@
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
       <c r="I24" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="J24" s="3" t="s">
-        <v>128</v>
-      </c>
+        <v>152</v>
+      </c>
+      <c r="J24" s="3"/>
       <c r="K24" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="L24" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="M24" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="L24" s="3" t="s">
+      <c r="N24" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="M24" s="3"/>
-      <c r="N24" s="3"/>
       <c r="O24" s="3"/>
-      <c r="P24" s="3" t="s">
+      <c r="P24" s="3"/>
+      <c r="Q24" s="3"/>
+      <c r="R24" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="Q24" s="3"/>
-      <c r="R24" s="3"/>
-      <c r="S24" s="3" t="s">
-        <v>139</v>
-      </c>
+      <c r="S24" s="3"/>
       <c r="T24" s="3"/>
-      <c r="U24" s="3"/>
+      <c r="U24" s="3" t="s">
+        <v>136</v>
+      </c>
       <c r="V24" s="3"/>
       <c r="W24" s="3"/>
       <c r="X24" s="3"/>
@@ -2887,8 +2951,10 @@
       <c r="AB24" s="3"/>
       <c r="AC24" s="3"/>
       <c r="AD24" s="3"/>
-    </row>
-    <row r="25" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AE24" s="3"/>
+      <c r="AF24" s="3"/>
+    </row>
+    <row r="25" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>105</v>
       </c>
@@ -2906,30 +2972,30 @@
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
       <c r="I25" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="J25" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="K25" s="3" t="s">
+      <c r="M25" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="L25" s="3" t="s">
+      <c r="N25" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="M25" s="3"/>
-      <c r="N25" s="3"/>
       <c r="O25" s="3"/>
-      <c r="P25" s="3" t="s">
-        <v>152</v>
-      </c>
+      <c r="P25" s="3"/>
       <c r="Q25" s="3"/>
-      <c r="R25" s="3"/>
-      <c r="S25" s="3" t="s">
-        <v>142</v>
-      </c>
+      <c r="R25" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="S25" s="3"/>
       <c r="T25" s="3"/>
-      <c r="U25" s="3"/>
+      <c r="U25" s="3" t="s">
+        <v>139</v>
+      </c>
       <c r="V25" s="3"/>
       <c r="W25" s="3"/>
       <c r="X25" s="3"/>
@@ -2939,8 +3005,10 @@
       <c r="AB25" s="3"/>
       <c r="AC25" s="3"/>
       <c r="AD25" s="3"/>
-    </row>
-    <row r="26" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AE25" s="3"/>
+      <c r="AF25" s="3"/>
+    </row>
+    <row r="26" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>105</v>
       </c>
@@ -2958,30 +3026,32 @@
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
       <c r="I26" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="J26" s="3" t="s">
-        <v>129</v>
-      </c>
+        <v>152</v>
+      </c>
+      <c r="J26" s="3"/>
       <c r="K26" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="L26" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="M26" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="L26" s="3" t="s">
+      <c r="N26" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="M26" s="3"/>
-      <c r="N26" s="3"/>
       <c r="O26" s="3"/>
-      <c r="P26" s="3" t="s">
-        <v>152</v>
-      </c>
+      <c r="P26" s="3"/>
       <c r="Q26" s="3"/>
-      <c r="R26" s="3"/>
-      <c r="S26" s="3" t="s">
+      <c r="R26" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="S26" s="3"/>
+      <c r="T26" s="3"/>
+      <c r="U26" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="T26" s="3"/>
-      <c r="U26" s="3"/>
       <c r="V26" s="3"/>
       <c r="W26" s="3"/>
       <c r="X26" s="3"/>
@@ -2991,8 +3061,10 @@
       <c r="AB26" s="3"/>
       <c r="AC26" s="3"/>
       <c r="AD26" s="3"/>
-    </row>
-    <row r="27" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AE26" s="3"/>
+      <c r="AF26" s="3"/>
+    </row>
+    <row r="27" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>105</v>
       </c>
@@ -3010,30 +3082,30 @@
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
       <c r="I27" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="J27" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="J27" s="3"/>
+      <c r="K27" s="3"/>
+      <c r="L27" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="K27" s="3" t="s">
+      <c r="M27" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="L27" s="3" t="s">
+      <c r="N27" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="M27" s="3"/>
-      <c r="N27" s="3"/>
       <c r="O27" s="3"/>
-      <c r="P27" s="3" t="s">
+      <c r="P27" s="3"/>
+      <c r="Q27" s="3"/>
+      <c r="R27" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="Q27" s="3"/>
-      <c r="R27" s="3"/>
-      <c r="S27" s="3" t="s">
-        <v>143</v>
-      </c>
+      <c r="S27" s="3"/>
       <c r="T27" s="3"/>
-      <c r="U27" s="3"/>
+      <c r="U27" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="V27" s="3"/>
       <c r="W27" s="3"/>
       <c r="X27" s="3"/>
@@ -3043,8 +3115,10 @@
       <c r="AB27" s="3"/>
       <c r="AC27" s="3"/>
       <c r="AD27" s="3"/>
-    </row>
-    <row r="28" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AE27" s="3"/>
+      <c r="AF27" s="3"/>
+    </row>
+    <row r="28" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>105</v>
       </c>
@@ -3062,30 +3136,30 @@
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
       <c r="I28" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="J28" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="J28" s="3"/>
+      <c r="K28" s="3"/>
+      <c r="L28" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="K28" s="3" t="s">
+      <c r="M28" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="L28" s="3" t="s">
+      <c r="N28" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="M28" s="3"/>
-      <c r="N28" s="3"/>
       <c r="O28" s="3"/>
-      <c r="P28" s="3" t="s">
-        <v>151</v>
-      </c>
+      <c r="P28" s="3"/>
       <c r="Q28" s="3"/>
-      <c r="R28" s="3"/>
-      <c r="S28" s="3" t="s">
+      <c r="R28" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="S28" s="3"/>
+      <c r="T28" s="3"/>
+      <c r="U28" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="T28" s="3"/>
-      <c r="U28" s="3"/>
       <c r="V28" s="3"/>
       <c r="W28" s="3"/>
       <c r="X28" s="3"/>
@@ -3095,8 +3169,10 @@
       <c r="AB28" s="3"/>
       <c r="AC28" s="3"/>
       <c r="AD28" s="3"/>
-    </row>
-    <row r="29" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AE28" s="3"/>
+      <c r="AF28" s="3"/>
+    </row>
+    <row r="29" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>105</v>
       </c>
@@ -3114,30 +3190,30 @@
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
       <c r="I29" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="J29" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="K29" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="J29" s="3"/>
+      <c r="K29" s="3"/>
+      <c r="L29" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="M29" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="L29" s="3" t="s">
+      <c r="N29" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="M29" s="3"/>
-      <c r="N29" s="3"/>
       <c r="O29" s="3"/>
-      <c r="P29" s="3" t="s">
-        <v>153</v>
-      </c>
+      <c r="P29" s="3"/>
       <c r="Q29" s="3"/>
-      <c r="R29" s="3"/>
-      <c r="S29" s="3" t="s">
-        <v>141</v>
-      </c>
+      <c r="R29" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="S29" s="3"/>
       <c r="T29" s="3"/>
-      <c r="U29" s="3"/>
+      <c r="U29" s="3" t="s">
+        <v>138</v>
+      </c>
       <c r="V29" s="3"/>
       <c r="W29" s="3"/>
       <c r="X29" s="3"/>
@@ -3147,8 +3223,10 @@
       <c r="AB29" s="3"/>
       <c r="AC29" s="3"/>
       <c r="AD29" s="3"/>
-    </row>
-    <row r="30" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AE29" s="3"/>
+      <c r="AF29" s="3"/>
+    </row>
+    <row r="30" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>105</v>
       </c>
@@ -3166,30 +3244,30 @@
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
       <c r="I30" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="J30" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="J30" s="3"/>
+      <c r="K30" s="3"/>
+      <c r="L30" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="K30" s="3" t="s">
+      <c r="M30" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="L30" s="3" t="s">
+      <c r="N30" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="M30" s="3"/>
-      <c r="N30" s="3"/>
       <c r="O30" s="3"/>
-      <c r="P30" s="3" t="s">
-        <v>151</v>
-      </c>
+      <c r="P30" s="3"/>
       <c r="Q30" s="3"/>
-      <c r="R30" s="3"/>
-      <c r="S30" s="3" t="s">
-        <v>144</v>
-      </c>
+      <c r="R30" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="S30" s="3"/>
       <c r="T30" s="3"/>
-      <c r="U30" s="3"/>
+      <c r="U30" s="3" t="s">
+        <v>141</v>
+      </c>
       <c r="V30" s="3"/>
       <c r="W30" s="3"/>
       <c r="X30" s="3"/>
@@ -3199,8 +3277,10 @@
       <c r="AB30" s="3"/>
       <c r="AC30" s="3"/>
       <c r="AD30" s="3"/>
-    </row>
-    <row r="31" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AE30" s="3"/>
+      <c r="AF30" s="3"/>
+    </row>
+    <row r="31" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>105</v>
       </c>
@@ -3218,30 +3298,30 @@
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
       <c r="I31" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="J31" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="J31" s="3"/>
+      <c r="K31" s="3"/>
+      <c r="L31" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="K31" s="3" t="s">
+      <c r="M31" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="L31" s="3" t="s">
+      <c r="N31" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="M31" s="3"/>
-      <c r="N31" s="3"/>
       <c r="O31" s="3"/>
-      <c r="P31" s="3" t="s">
-        <v>153</v>
-      </c>
+      <c r="P31" s="3"/>
       <c r="Q31" s="3"/>
-      <c r="R31" s="3"/>
-      <c r="S31" s="3" t="s">
-        <v>145</v>
-      </c>
+      <c r="R31" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="S31" s="3"/>
       <c r="T31" s="3"/>
-      <c r="U31" s="3"/>
+      <c r="U31" s="3" t="s">
+        <v>142</v>
+      </c>
       <c r="V31" s="3"/>
       <c r="W31" s="3"/>
       <c r="X31" s="3"/>
@@ -3251,8 +3331,10 @@
       <c r="AB31" s="3"/>
       <c r="AC31" s="3"/>
       <c r="AD31" s="3"/>
-    </row>
-    <row r="32" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AE31" s="3"/>
+      <c r="AF31" s="3"/>
+    </row>
+    <row r="32" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>105</v>
       </c>
@@ -3270,30 +3352,30 @@
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
       <c r="I32" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="J32" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="J32" s="3"/>
+      <c r="K32" s="3"/>
+      <c r="L32" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="K32" s="3" t="s">
+      <c r="M32" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="L32" s="3" t="s">
+      <c r="N32" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="M32" s="3"/>
-      <c r="N32" s="3"/>
       <c r="O32" s="3"/>
-      <c r="P32" s="3" t="s">
-        <v>76</v>
-      </c>
+      <c r="P32" s="3"/>
       <c r="Q32" s="3"/>
-      <c r="R32" s="3"/>
-      <c r="S32" s="3" t="s">
+      <c r="R32" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="S32" s="3"/>
+      <c r="T32" s="3"/>
+      <c r="U32" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="T32" s="3"/>
-      <c r="U32" s="3"/>
       <c r="V32" s="3"/>
       <c r="W32" s="3"/>
       <c r="X32" s="3"/>
@@ -3303,8 +3385,10 @@
       <c r="AB32" s="3"/>
       <c r="AC32" s="3"/>
       <c r="AD32" s="3"/>
-    </row>
-    <row r="33" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AE32" s="3"/>
+      <c r="AF32" s="3"/>
+    </row>
+    <row r="33" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>105</v>
       </c>
@@ -3322,30 +3406,34 @@
       <c r="G33" s="3"/>
       <c r="H33" s="3"/>
       <c r="I33" s="3" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="J33" s="3" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="K33" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="L33" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="M33" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="L33" s="3" t="s">
+      <c r="N33" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="M33" s="3"/>
-      <c r="N33" s="3"/>
       <c r="O33" s="3"/>
-      <c r="P33" s="3" t="s">
-        <v>76</v>
-      </c>
+      <c r="P33" s="3"/>
       <c r="Q33" s="3"/>
-      <c r="R33" s="3"/>
-      <c r="S33" s="3" t="s">
-        <v>146</v>
-      </c>
+      <c r="R33" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="S33" s="3"/>
       <c r="T33" s="3"/>
-      <c r="U33" s="3"/>
+      <c r="U33" s="3" t="s">
+        <v>143</v>
+      </c>
       <c r="V33" s="3"/>
       <c r="W33" s="3"/>
       <c r="X33" s="3"/>
@@ -3355,8 +3443,10 @@
       <c r="AB33" s="3"/>
       <c r="AC33" s="3"/>
       <c r="AD33" s="3"/>
-    </row>
-    <row r="34" spans="1:30" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AE33" s="3"/>
+      <c r="AF33" s="3"/>
+    </row>
+    <row r="34" spans="1:32" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="3">
         <v>1148</v>
       </c>
@@ -3364,16 +3454,16 @@
         <v>89</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="G34" s="3"/>
       <c r="H34" s="3"/>
@@ -3382,37 +3472,39 @@
       <c r="K34" s="3"/>
       <c r="L34" s="3"/>
       <c r="M34" s="3"/>
-      <c r="N34" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="O34" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="P34" s="3"/>
-      <c r="Q34" s="3"/>
-      <c r="R34" s="3" t="s">
-        <v>173</v>
-      </c>
+      <c r="N34" s="3"/>
+      <c r="O34" s="3"/>
+      <c r="P34" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="Q34" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="R34" s="3"/>
       <c r="S34" s="3"/>
-      <c r="T34" s="3"/>
-      <c r="U34" s="3" t="s">
+      <c r="T34" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="U34" s="3"/>
+      <c r="V34" s="3"/>
+      <c r="W34" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="V34" s="3"/>
-      <c r="W34" s="3"/>
-      <c r="X34" s="3" t="s">
-        <v>145</v>
-      </c>
+      <c r="X34" s="3"/>
       <c r="Y34" s="3"/>
       <c r="Z34" s="3" t="s">
-        <v>187</v>
+        <v>142</v>
       </c>
       <c r="AA34" s="3"/>
-      <c r="AB34" s="3"/>
+      <c r="AB34" s="3" t="s">
+        <v>184</v>
+      </c>
       <c r="AC34" s="3"/>
       <c r="AD34" s="3"/>
-    </row>
-    <row r="35" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AE34" s="3"/>
+      <c r="AF34" s="3"/>
+    </row>
+    <row r="35" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A35" s="3">
         <v>1148</v>
       </c>
@@ -3420,16 +3512,16 @@
         <v>89</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>76</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="G35" s="3"/>
       <c r="H35" s="3"/>
@@ -3438,37 +3530,39 @@
       <c r="K35" s="3"/>
       <c r="L35" s="3"/>
       <c r="M35" s="3"/>
-      <c r="N35" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="O35" s="3" t="s">
+      <c r="N35" s="3"/>
+      <c r="O35" s="3"/>
+      <c r="P35" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="Q35" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="P35" s="3"/>
-      <c r="Q35" s="3"/>
-      <c r="R35" s="3" t="s">
-        <v>174</v>
-      </c>
+      <c r="R35" s="3"/>
       <c r="S35" s="3"/>
-      <c r="T35" s="3"/>
-      <c r="U35" s="3" t="s">
-        <v>76</v>
-      </c>
+      <c r="T35" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="U35" s="3"/>
       <c r="V35" s="3"/>
-      <c r="W35" s="3"/>
-      <c r="X35" s="3" t="s">
-        <v>76</v>
-      </c>
+      <c r="W35" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="X35" s="3"/>
       <c r="Y35" s="3"/>
       <c r="Z35" s="3" t="s">
         <v>76</v>
       </c>
       <c r="AA35" s="3"/>
-      <c r="AB35" s="3"/>
+      <c r="AB35" s="3" t="s">
+        <v>76</v>
+      </c>
       <c r="AC35" s="3"/>
       <c r="AD35" s="3"/>
-    </row>
-    <row r="36" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AE35" s="3"/>
+      <c r="AF35" s="3"/>
+    </row>
+    <row r="36" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A36" s="3">
         <v>1148</v>
       </c>
@@ -3476,14 +3570,14 @@
         <v>89</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E36" s="3"/>
       <c r="F36" s="3" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
@@ -3492,37 +3586,39 @@
       <c r="K36" s="3"/>
       <c r="L36" s="3"/>
       <c r="M36" s="3"/>
-      <c r="N36" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="O36" s="3" t="s">
+      <c r="N36" s="3"/>
+      <c r="O36" s="3"/>
+      <c r="P36" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="Q36" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="P36" s="3"/>
-      <c r="Q36" s="3"/>
-      <c r="R36" s="3" t="s">
-        <v>175</v>
-      </c>
+      <c r="R36" s="3"/>
       <c r="S36" s="3"/>
-      <c r="T36" s="3"/>
-      <c r="U36" s="3" t="s">
+      <c r="T36" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="U36" s="3"/>
+      <c r="V36" s="3"/>
+      <c r="W36" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="V36" s="3"/>
-      <c r="W36" s="3"/>
-      <c r="X36" s="3" t="s">
-        <v>76</v>
-      </c>
+      <c r="X36" s="3"/>
       <c r="Y36" s="3"/>
       <c r="Z36" s="3" t="s">
-        <v>188</v>
+        <v>76</v>
       </c>
       <c r="AA36" s="3"/>
-      <c r="AB36" s="3"/>
+      <c r="AB36" s="3" t="s">
+        <v>185</v>
+      </c>
       <c r="AC36" s="3"/>
       <c r="AD36" s="3"/>
-    </row>
-    <row r="37" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AE36" s="3"/>
+      <c r="AF36" s="3"/>
+    </row>
+    <row r="37" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A37" s="3">
         <v>1148</v>
       </c>
@@ -3530,10 +3626,10 @@
         <v>89</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E37" s="3"/>
       <c r="F37" s="3" t="s">
@@ -3546,37 +3642,39 @@
       <c r="K37" s="3"/>
       <c r="L37" s="3"/>
       <c r="M37" s="3"/>
-      <c r="N37" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="O37" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="P37" s="3"/>
-      <c r="Q37" s="3"/>
-      <c r="R37" s="3" t="s">
-        <v>176</v>
-      </c>
+      <c r="N37" s="3"/>
+      <c r="O37" s="3"/>
+      <c r="P37" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q37" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="R37" s="3"/>
       <c r="S37" s="3"/>
-      <c r="T37" s="3"/>
-      <c r="U37" s="3" t="s">
+      <c r="T37" s="3" t="s">
         <v>173</v>
       </c>
+      <c r="U37" s="3"/>
       <c r="V37" s="3"/>
-      <c r="W37" s="3"/>
-      <c r="X37" s="3" t="s">
-        <v>182</v>
-      </c>
+      <c r="W37" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="X37" s="3"/>
       <c r="Y37" s="3"/>
       <c r="Z37" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="AA37" s="3"/>
+      <c r="AB37" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="AA37" s="3"/>
-      <c r="AB37" s="3"/>
       <c r="AC37" s="3"/>
       <c r="AD37" s="3"/>
-    </row>
-    <row r="38" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AE37" s="3"/>
+      <c r="AF37" s="3"/>
+    </row>
+    <row r="38" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A38" s="3">
         <v>1148</v>
       </c>
@@ -3584,16 +3682,16 @@
         <v>89</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="G38" s="3"/>
       <c r="H38" s="3"/>
@@ -3602,37 +3700,39 @@
       <c r="K38" s="3"/>
       <c r="L38" s="3"/>
       <c r="M38" s="3"/>
-      <c r="N38" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="O38" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="P38" s="3"/>
-      <c r="Q38" s="3"/>
-      <c r="R38" s="3" t="s">
-        <v>177</v>
-      </c>
+      <c r="N38" s="3"/>
+      <c r="O38" s="3"/>
+      <c r="P38" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="Q38" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="R38" s="3"/>
       <c r="S38" s="3"/>
-      <c r="T38" s="3"/>
-      <c r="U38" s="3" t="s">
-        <v>192</v>
-      </c>
+      <c r="T38" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="U38" s="3"/>
       <c r="V38" s="3"/>
-      <c r="W38" s="3"/>
-      <c r="X38" s="3" t="s">
-        <v>183</v>
-      </c>
+      <c r="W38" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="X38" s="3"/>
       <c r="Y38" s="3"/>
       <c r="Z38" s="3" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="AA38" s="3"/>
-      <c r="AB38" s="3"/>
+      <c r="AB38" s="3" t="s">
+        <v>180</v>
+      </c>
       <c r="AC38" s="3"/>
       <c r="AD38" s="3"/>
-    </row>
-    <row r="39" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AE38" s="3"/>
+      <c r="AF38" s="3"/>
+    </row>
+    <row r="39" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A39" s="3">
         <v>1148</v>
       </c>
@@ -3640,16 +3740,16 @@
         <v>89</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="G39" s="3"/>
       <c r="H39" s="3"/>
@@ -3658,39 +3758,41 @@
       <c r="K39" s="3"/>
       <c r="L39" s="3"/>
       <c r="M39" s="3"/>
-      <c r="N39" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="O39" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="P39" s="3"/>
-      <c r="Q39" s="3"/>
-      <c r="R39" s="3" t="s">
-        <v>178</v>
-      </c>
+      <c r="N39" s="3"/>
+      <c r="O39" s="3"/>
+      <c r="P39" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="Q39" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="R39" s="3"/>
       <c r="S39" s="3"/>
-      <c r="T39" s="3"/>
-      <c r="U39" s="3" t="s">
-        <v>139</v>
-      </c>
+      <c r="T39" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="U39" s="3"/>
       <c r="V39" s="3"/>
-      <c r="W39" s="3"/>
-      <c r="X39" s="3" t="s">
-        <v>76</v>
-      </c>
+      <c r="W39" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="X39" s="3"/>
       <c r="Y39" s="3"/>
       <c r="Z39" s="3" t="s">
-        <v>189</v>
+        <v>76</v>
       </c>
       <c r="AA39" s="3"/>
-      <c r="AB39" s="3"/>
+      <c r="AB39" s="3" t="s">
+        <v>186</v>
+      </c>
       <c r="AC39" s="3"/>
-      <c r="AD39" s="3" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="40" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AD39" s="3"/>
+      <c r="AE39" s="3"/>
+      <c r="AF39" s="3" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="40" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A40" s="3">
         <v>1148</v>
       </c>
@@ -3698,16 +3800,16 @@
         <v>89</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="G40" s="3"/>
       <c r="H40" s="3"/>
@@ -3716,39 +3818,41 @@
       <c r="K40" s="3"/>
       <c r="L40" s="3"/>
       <c r="M40" s="3"/>
-      <c r="N40" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="O40" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="P40" s="3"/>
-      <c r="Q40" s="3"/>
-      <c r="R40" s="3" t="s">
-        <v>179</v>
-      </c>
+      <c r="N40" s="3"/>
+      <c r="O40" s="3"/>
+      <c r="P40" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="Q40" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="R40" s="3"/>
       <c r="S40" s="3"/>
-      <c r="T40" s="3"/>
-      <c r="U40" s="3" t="s">
-        <v>196</v>
-      </c>
+      <c r="T40" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="U40" s="3"/>
       <c r="V40" s="3"/>
-      <c r="W40" s="3"/>
-      <c r="X40" s="3" t="s">
-        <v>76</v>
-      </c>
+      <c r="W40" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="X40" s="3"/>
       <c r="Y40" s="3"/>
       <c r="Z40" s="3" t="s">
-        <v>140</v>
+        <v>76</v>
       </c>
       <c r="AA40" s="3"/>
-      <c r="AB40" s="3"/>
+      <c r="AB40" s="3" t="s">
+        <v>137</v>
+      </c>
       <c r="AC40" s="3"/>
-      <c r="AD40" s="3" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="41" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AD40" s="3"/>
+      <c r="AE40" s="3"/>
+      <c r="AF40" s="3" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="41" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A41" s="3">
         <v>1148</v>
       </c>
@@ -3756,16 +3860,16 @@
         <v>89</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="G41" s="3"/>
       <c r="H41" s="3"/>
@@ -3774,39 +3878,41 @@
       <c r="K41" s="3"/>
       <c r="L41" s="3"/>
       <c r="M41" s="3"/>
-      <c r="N41" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="O41" s="3" t="s">
+      <c r="N41" s="3"/>
+      <c r="O41" s="3"/>
+      <c r="P41" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="Q41" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="P41" s="3"/>
-      <c r="Q41" s="3"/>
-      <c r="R41" s="3" t="s">
-        <v>180</v>
-      </c>
+      <c r="R41" s="3"/>
       <c r="S41" s="3"/>
-      <c r="T41" s="3"/>
-      <c r="U41" s="3" t="s">
-        <v>192</v>
-      </c>
+      <c r="T41" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="U41" s="3"/>
       <c r="V41" s="3"/>
-      <c r="W41" s="3"/>
-      <c r="X41" s="3" t="s">
-        <v>76</v>
-      </c>
+      <c r="W41" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="X41" s="3"/>
       <c r="Y41" s="3"/>
       <c r="Z41" s="3" t="s">
-        <v>182</v>
+        <v>76</v>
       </c>
       <c r="AA41" s="3"/>
-      <c r="AB41" s="3"/>
+      <c r="AB41" s="3" t="s">
+        <v>179</v>
+      </c>
       <c r="AC41" s="3"/>
-      <c r="AD41" s="3" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="42" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AD41" s="3"/>
+      <c r="AE41" s="3"/>
+      <c r="AF41" s="3" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="42" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A42" s="3">
         <v>1148</v>
       </c>
@@ -3814,14 +3920,14 @@
         <v>89</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="E42" s="3"/>
       <c r="F42" s="3" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="G42" s="3"/>
       <c r="H42" s="3"/>
@@ -3830,37 +3936,39 @@
       <c r="K42" s="3"/>
       <c r="L42" s="3"/>
       <c r="M42" s="3"/>
-      <c r="N42" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="O42" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="P42" s="3"/>
-      <c r="Q42" s="3"/>
-      <c r="R42" s="3" t="s">
-        <v>181</v>
-      </c>
+      <c r="N42" s="3"/>
+      <c r="O42" s="3"/>
+      <c r="P42" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q42" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="R42" s="3"/>
       <c r="S42" s="3"/>
-      <c r="T42" s="3"/>
-      <c r="U42" s="3" t="s">
-        <v>76</v>
-      </c>
+      <c r="T42" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="U42" s="3"/>
       <c r="V42" s="3"/>
-      <c r="W42" s="3"/>
-      <c r="X42" s="3" t="s">
-        <v>76</v>
-      </c>
+      <c r="W42" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="X42" s="3"/>
       <c r="Y42" s="3"/>
       <c r="Z42" s="3" t="s">
         <v>76</v>
       </c>
       <c r="AA42" s="3"/>
-      <c r="AB42" s="3"/>
+      <c r="AB42" s="3" t="s">
+        <v>76</v>
+      </c>
       <c r="AC42" s="3"/>
       <c r="AD42" s="3"/>
-    </row>
-    <row r="43" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AE42" s="3"/>
+      <c r="AF42" s="3"/>
+    </row>
+    <row r="43" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A43" s="3">
         <v>1148</v>
       </c>
@@ -3868,14 +3976,14 @@
         <v>89</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="E43" s="3"/>
       <c r="F43" s="3" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="G43" s="3"/>
       <c r="H43" s="3"/>
@@ -3884,37 +3992,39 @@
       <c r="K43" s="3"/>
       <c r="L43" s="3"/>
       <c r="M43" s="3"/>
-      <c r="N43" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="O43" s="3" t="s">
+      <c r="N43" s="3"/>
+      <c r="O43" s="3"/>
+      <c r="P43" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="Q43" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="P43" s="3"/>
-      <c r="Q43" s="3"/>
-      <c r="R43" s="3" t="s">
-        <v>175</v>
-      </c>
+      <c r="R43" s="3"/>
       <c r="S43" s="3"/>
-      <c r="T43" s="3"/>
-      <c r="U43" s="3" t="s">
+      <c r="T43" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="U43" s="3"/>
+      <c r="V43" s="3"/>
+      <c r="W43" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="V43" s="3"/>
-      <c r="W43" s="3"/>
-      <c r="X43" s="3" t="s">
-        <v>76</v>
-      </c>
+      <c r="X43" s="3"/>
       <c r="Y43" s="3"/>
       <c r="Z43" s="3" t="s">
-        <v>190</v>
+        <v>76</v>
       </c>
       <c r="AA43" s="3"/>
-      <c r="AB43" s="3"/>
+      <c r="AB43" s="3" t="s">
+        <v>187</v>
+      </c>
       <c r="AC43" s="3"/>
       <c r="AD43" s="3"/>
-    </row>
-    <row r="44" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AE43" s="3"/>
+      <c r="AF43" s="3"/>
+    </row>
+    <row r="44" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A44" s="3">
         <v>1148</v>
       </c>
@@ -3922,14 +4032,14 @@
         <v>89</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="E44" s="3"/>
       <c r="F44" s="3" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="G44" s="3"/>
       <c r="H44" s="3"/>
@@ -3938,37 +4048,39 @@
       <c r="K44" s="3"/>
       <c r="L44" s="3"/>
       <c r="M44" s="3"/>
-      <c r="N44" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="O44" s="3" t="s">
+      <c r="N44" s="3"/>
+      <c r="O44" s="3"/>
+      <c r="P44" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="Q44" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="P44" s="3"/>
-      <c r="Q44" s="3"/>
-      <c r="R44" s="3" t="s">
-        <v>179</v>
-      </c>
+      <c r="R44" s="3"/>
       <c r="S44" s="3"/>
-      <c r="T44" s="3"/>
-      <c r="U44" s="3" t="s">
-        <v>141</v>
-      </c>
+      <c r="T44" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="U44" s="3"/>
       <c r="V44" s="3"/>
-      <c r="W44" s="3"/>
-      <c r="X44" s="3" t="s">
-        <v>182</v>
-      </c>
+      <c r="W44" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="X44" s="3"/>
       <c r="Y44" s="3"/>
       <c r="Z44" s="3" t="s">
-        <v>145</v>
+        <v>179</v>
       </c>
       <c r="AA44" s="3"/>
-      <c r="AB44" s="3"/>
+      <c r="AB44" s="3" t="s">
+        <v>142</v>
+      </c>
       <c r="AC44" s="3"/>
       <c r="AD44" s="3"/>
-    </row>
-    <row r="45" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AE44" s="3"/>
+      <c r="AF44" s="3"/>
+    </row>
+    <row r="45" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A45" s="3">
         <v>1148</v>
       </c>
@@ -3976,14 +4088,14 @@
         <v>89</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="E45" s="3"/>
       <c r="F45" s="3" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="G45" s="3"/>
       <c r="H45" s="3"/>
@@ -3992,37 +4104,39 @@
       <c r="K45" s="3"/>
       <c r="L45" s="3"/>
       <c r="M45" s="3"/>
-      <c r="N45" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="O45" s="3" t="s">
+      <c r="N45" s="3"/>
+      <c r="O45" s="3"/>
+      <c r="P45" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="Q45" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="P45" s="3"/>
-      <c r="Q45" s="3"/>
-      <c r="R45" s="3" t="s">
+      <c r="R45" s="3"/>
+      <c r="S45" s="3"/>
+      <c r="T45" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="S45" s="3"/>
-      <c r="T45" s="3"/>
-      <c r="U45" s="3" t="s">
+      <c r="U45" s="3"/>
+      <c r="V45" s="3"/>
+      <c r="W45" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="V45" s="3"/>
-      <c r="W45" s="3"/>
-      <c r="X45" s="3" t="s">
-        <v>184</v>
-      </c>
+      <c r="X45" s="3"/>
       <c r="Y45" s="3"/>
       <c r="Z45" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="AA45" s="3"/>
-      <c r="AB45" s="3"/>
+      <c r="AB45" s="3" t="s">
+        <v>188</v>
+      </c>
       <c r="AC45" s="3"/>
       <c r="AD45" s="3"/>
-    </row>
-    <row r="46" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AE45" s="3"/>
+      <c r="AF45" s="3"/>
+    </row>
+    <row r="46" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A46" s="3">
         <v>1148</v>
       </c>
@@ -4030,14 +4144,14 @@
         <v>89</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="E46" s="3"/>
       <c r="F46" s="3" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="G46" s="3"/>
       <c r="H46" s="3"/>
@@ -4046,37 +4160,39 @@
       <c r="K46" s="3"/>
       <c r="L46" s="3"/>
       <c r="M46" s="3"/>
-      <c r="N46" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="O46" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="P46" s="3"/>
-      <c r="Q46" s="3"/>
-      <c r="R46" s="3" t="s">
-        <v>179</v>
-      </c>
+      <c r="N46" s="3"/>
+      <c r="O46" s="3"/>
+      <c r="P46" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="Q46" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="R46" s="3"/>
       <c r="S46" s="3"/>
-      <c r="T46" s="3"/>
-      <c r="U46" s="3" t="s">
+      <c r="T46" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="U46" s="3"/>
+      <c r="V46" s="3"/>
+      <c r="W46" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="V46" s="3"/>
-      <c r="W46" s="3"/>
-      <c r="X46" s="3" t="s">
-        <v>185</v>
-      </c>
+      <c r="X46" s="3"/>
       <c r="Y46" s="3"/>
       <c r="Z46" s="3" t="s">
-        <v>139</v>
+        <v>182</v>
       </c>
       <c r="AA46" s="3"/>
-      <c r="AB46" s="3"/>
+      <c r="AB46" s="3" t="s">
+        <v>136</v>
+      </c>
       <c r="AC46" s="3"/>
       <c r="AD46" s="3"/>
-    </row>
-    <row r="47" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AE46" s="3"/>
+      <c r="AF46" s="3"/>
+    </row>
+    <row r="47" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A47" s="3">
         <v>1148</v>
       </c>
@@ -4084,14 +4200,14 @@
         <v>89</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="E47" s="3"/>
       <c r="F47" s="3" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="G47" s="3"/>
       <c r="H47" s="3"/>
@@ -4100,35 +4216,37 @@
       <c r="K47" s="3"/>
       <c r="L47" s="3"/>
       <c r="M47" s="3"/>
-      <c r="N47" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="O47" s="3" t="s">
+      <c r="N47" s="3"/>
+      <c r="O47" s="3"/>
+      <c r="P47" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="Q47" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="P47" s="3"/>
-      <c r="Q47" s="3"/>
-      <c r="R47" s="3" t="s">
-        <v>179</v>
-      </c>
+      <c r="R47" s="3"/>
       <c r="S47" s="3"/>
-      <c r="T47" s="3"/>
-      <c r="U47" s="3" t="s">
-        <v>197</v>
-      </c>
+      <c r="T47" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="U47" s="3"/>
       <c r="V47" s="3"/>
-      <c r="W47" s="3"/>
-      <c r="X47" s="3" t="s">
-        <v>186</v>
-      </c>
+      <c r="W47" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="X47" s="3"/>
       <c r="Y47" s="3"/>
       <c r="Z47" s="3" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="AA47" s="3"/>
-      <c r="AB47" s="3"/>
+      <c r="AB47" s="3" t="s">
+        <v>187</v>
+      </c>
       <c r="AC47" s="3"/>
       <c r="AD47" s="3"/>
+      <c r="AE47" s="3"/>
+      <c r="AF47" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
finished updating to new template
</commit_message>
<xml_diff>
--- a/analyses/scrapeUSDAseedmanual/scraping/usdaDataScraping_CRD.xlsx
+++ b/analyses/scrapeUSDAseedmanual/scraping/usdaDataScraping_CRD.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10511"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christophe_rouleau-desrochers/github/egret/analyses/scrapeUSDAseedmanual/scraping/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1867F29B-ADA1-0B4D-ACB0-E1BD7483F99A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8165CA8D-1D56-6D41-9812-B527799553BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29400" yWindow="-2480" windowWidth="38400" windowHeight="21600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Meta" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="215">
   <si>
     <t>pdf_page_number</t>
   </si>
@@ -696,16 +696,17 @@
     <t>47 to 61</t>
   </si>
   <si>
-    <t>warm_stratification_days2</t>
-  </si>
-  <si>
     <t>warm_stratification_temp_C</t>
   </si>
   <si>
+    <t>25</t>
+  </si>
+  <si>
     <t>cold_stratification_temp_C</t>
-  </si>
-  <si>
-    <t>25</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>prechilling given in text, no details on temperature</t>
   </si>
 </sst>
 </file>
@@ -898,28 +899,28 @@
     <tableColumn id="8" xr3:uid="{25D42B2B-7F05-4140-A3C6-F8B396550CAB}" name="pregermination_treatment_hot_water_soak_C" dataDxfId="24"/>
     <tableColumn id="9" xr3:uid="{55A4F340-7B6D-7943-8B39-CFAE9E6FE33F}" name="pretreatment" dataDxfId="23"/>
     <tableColumn id="10" xr3:uid="{4A6EEDC6-97D1-5C4D-8AA2-6F5DFBF4D1C4}" name="stratification_temp_C" dataDxfId="22"/>
-    <tableColumn id="31" xr3:uid="{C2EB3AFD-A023-9943-99AC-88FDB5F21DAA}" name="warm_stratification_temp_C" dataDxfId="1"/>
-    <tableColumn id="32" xr3:uid="{722DB568-4A1B-2143-82BA-AA33796FD61E}" name="cold_stratification_temp_C" dataDxfId="0"/>
-    <tableColumn id="11" xr3:uid="{DEEF428E-8BC4-ED4F-A0A2-906B50FA71DD}" name="warm_stratification_days2" dataDxfId="21"/>
-    <tableColumn id="12" xr3:uid="{93B28E55-01FC-F64C-9809-1780CA274A58}" name="cold_stratification_days" dataDxfId="20"/>
-    <tableColumn id="13" xr3:uid="{FBA71BC1-6F33-B742-9505-31E5F69BC022}" name="dailyl_light_hours" dataDxfId="19"/>
-    <tableColumn id="14" xr3:uid="{B60543C3-E2EE-A64E-A396-1C242453800C}" name="day_temp_celsius" dataDxfId="18"/>
-    <tableColumn id="15" xr3:uid="{A98F0563-6BD3-C049-89CC-CCFA69D88415}" name="night_temp_celsius" dataDxfId="17"/>
-    <tableColumn id="16" xr3:uid="{441701F9-64D9-6C4C-98DD-50E953D9AE81}" name="temp_unspecified_time_of_day_celsius" dataDxfId="16"/>
-    <tableColumn id="17" xr3:uid="{8E32E59C-2511-5E47-B942-01EF1C2F823C}" name="test_duration_in_days" dataDxfId="15"/>
-    <tableColumn id="18" xr3:uid="{427BB247-5A32-DE42-AC51-6837CDABE181}" name="germination_time_days" dataDxfId="14"/>
-    <tableColumn id="19" xr3:uid="{35DE5AFC-901F-3445-96DA-507E967B4ECB}" name="total_germination_percent" dataDxfId="13"/>
-    <tableColumn id="20" xr3:uid="{BC769C61-E4F8-114A-B837-872ED1FFEAAC}" name="avg_germination_percent" dataDxfId="12"/>
-    <tableColumn id="21" xr3:uid="{093E7249-8AC3-8044-8840-C1350D4C13FA}" name="samples" dataDxfId="11"/>
-    <tableColumn id="22" xr3:uid="{4AAA545E-A06B-5A49-A9C2-811A91D56309}" name="germination_rate" dataDxfId="10"/>
-    <tableColumn id="23" xr3:uid="{0E3380FC-04AB-B648-BA64-33C0172712E8}" name="avg_germinative_energy_percent" dataDxfId="9"/>
-    <tableColumn id="24" xr3:uid="{BB029E85-4EEF-7541-A8A6-B78FC45AA990}" name="germinative_energy_percent" dataDxfId="8"/>
-    <tableColumn id="25" xr3:uid="{D9A90743-B6FB-BA4B-951F-4B5A9FC761BA}" name="avg_germinative_capacity" dataDxfId="7"/>
-    <tableColumn id="26" xr3:uid="{5AE4612B-E138-4D40-8419-CC14A92B62CD}" name="germinative_capacity" dataDxfId="6"/>
-    <tableColumn id="27" xr3:uid="{5BE09F3B-7D66-884A-B192-CEE49F2B845E}" name="percent_germination_15degC_incubated" dataDxfId="5"/>
-    <tableColumn id="28" xr3:uid="{6061511F-2CE6-FF4C-BA21-079020EC6884}" name="percent_germination_20degC_incubated" dataDxfId="4"/>
-    <tableColumn id="29" xr3:uid="{B17A6158-E57A-8B49-B7C6-A792A8BB3857}" name="50%_germ" dataDxfId="3"/>
-    <tableColumn id="30" xr3:uid="{C6852079-746D-E843-96F0-451DDB3F34C3}" name="Notes" dataDxfId="2"/>
+    <tableColumn id="33" xr3:uid="{1210F0BD-23B5-9140-8426-31FF90F8FB3C}" name="warm_stratification_temp_C" dataDxfId="3"/>
+    <tableColumn id="36" xr3:uid="{E51E641D-9B06-5E4C-9658-7002B1B1CEF1}" name="warm_stratification_days" dataDxfId="1"/>
+    <tableColumn id="35" xr3:uid="{FD04900B-878E-AC42-911D-9C9BE08CE010}" name="cold_stratification_temp_C" dataDxfId="2"/>
+    <tableColumn id="34" xr3:uid="{3E825D95-CDE2-874E-89AF-5DD665872E8B}" name="cold_stratification_days" dataDxfId="0"/>
+    <tableColumn id="13" xr3:uid="{FBA71BC1-6F33-B742-9505-31E5F69BC022}" name="dailyl_light_hours" dataDxfId="21"/>
+    <tableColumn id="14" xr3:uid="{B60543C3-E2EE-A64E-A396-1C242453800C}" name="day_temp_celsius" dataDxfId="20"/>
+    <tableColumn id="15" xr3:uid="{A98F0563-6BD3-C049-89CC-CCFA69D88415}" name="night_temp_celsius" dataDxfId="19"/>
+    <tableColumn id="16" xr3:uid="{441701F9-64D9-6C4C-98DD-50E953D9AE81}" name="temp_unspecified_time_of_day_celsius" dataDxfId="18"/>
+    <tableColumn id="17" xr3:uid="{8E32E59C-2511-5E47-B942-01EF1C2F823C}" name="test_duration_in_days" dataDxfId="17"/>
+    <tableColumn id="18" xr3:uid="{427BB247-5A32-DE42-AC51-6837CDABE181}" name="germination_time_days" dataDxfId="16"/>
+    <tableColumn id="19" xr3:uid="{35DE5AFC-901F-3445-96DA-507E967B4ECB}" name="total_germination_percent" dataDxfId="15"/>
+    <tableColumn id="20" xr3:uid="{BC769C61-E4F8-114A-B837-872ED1FFEAAC}" name="avg_germination_percent" dataDxfId="14"/>
+    <tableColumn id="21" xr3:uid="{093E7249-8AC3-8044-8840-C1350D4C13FA}" name="samples" dataDxfId="13"/>
+    <tableColumn id="22" xr3:uid="{4AAA545E-A06B-5A49-A9C2-811A91D56309}" name="germination_rate" dataDxfId="12"/>
+    <tableColumn id="23" xr3:uid="{0E3380FC-04AB-B648-BA64-33C0172712E8}" name="avg_germinative_energy_percent" dataDxfId="11"/>
+    <tableColumn id="24" xr3:uid="{BB029E85-4EEF-7541-A8A6-B78FC45AA990}" name="germinative_energy_percent" dataDxfId="10"/>
+    <tableColumn id="25" xr3:uid="{D9A90743-B6FB-BA4B-951F-4B5A9FC761BA}" name="avg_germinative_capacity" dataDxfId="9"/>
+    <tableColumn id="26" xr3:uid="{5AE4612B-E138-4D40-8419-CC14A92B62CD}" name="germinative_capacity" dataDxfId="8"/>
+    <tableColumn id="27" xr3:uid="{5BE09F3B-7D66-884A-B192-CEE49F2B845E}" name="percent_germination_15degC_incubated" dataDxfId="7"/>
+    <tableColumn id="28" xr3:uid="{6061511F-2CE6-FF4C-BA21-079020EC6884}" name="percent_germination_20degC_incubated" dataDxfId="6"/>
+    <tableColumn id="29" xr3:uid="{B17A6158-E57A-8B49-B7C6-A792A8BB3857}" name="50%_germ" dataDxfId="5"/>
+    <tableColumn id="30" xr3:uid="{C6852079-746D-E843-96F0-451DDB3F34C3}" name="Notes" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1513,8 +1514,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4AC4DDB-17EE-463A-9304-F699F6DBC2E2}">
   <dimension ref="A1:AF47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="187" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" topLeftCell="T14" zoomScale="125" workbookViewId="0">
+      <selection activeCell="AF8" sqref="AF8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1528,9 +1529,7 @@
     <col min="8" max="8" width="37.1640625" customWidth="1"/>
     <col min="9" max="9" width="12" customWidth="1"/>
     <col min="10" max="10" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="20.5" customWidth="1"/>
-    <col min="13" max="13" width="23" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="22" bestFit="1" customWidth="1"/>
+    <col min="11" max="14" width="20.5" customWidth="1"/>
     <col min="15" max="15" width="15.5" customWidth="1"/>
     <col min="16" max="16" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="18.83203125" bestFit="1" customWidth="1"/>
@@ -1582,13 +1581,13 @@
         <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>213</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>211</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>11</v>
@@ -2012,7 +2011,9 @@
       <c r="AC7" s="3"/>
       <c r="AD7" s="3"/>
       <c r="AE7" s="3"/>
-      <c r="AF7" s="3"/>
+      <c r="AF7" s="3" t="s">
+        <v>214</v>
+      </c>
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
@@ -2097,10 +2098,10 @@
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
       <c r="L9" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="M9" s="3" t="s">
         <v>124</v>
-      </c>
-      <c r="M9" s="3" t="s">
-        <v>123</v>
       </c>
       <c r="N9" s="3" t="s">
         <v>114</v>
@@ -2152,13 +2153,13 @@
       </c>
       <c r="J10" s="3"/>
       <c r="K10" s="3" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="L10" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="M10" s="3" t="s">
         <v>124</v>
-      </c>
-      <c r="M10" s="3" t="s">
-        <v>110</v>
       </c>
       <c r="N10" s="3" t="s">
         <v>112</v>
@@ -2211,10 +2212,10 @@
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
       <c r="L11" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="M11" s="3" t="s">
         <v>124</v>
-      </c>
-      <c r="M11" s="3" t="s">
-        <v>123</v>
       </c>
       <c r="N11" s="3" t="s">
         <v>112</v>
@@ -2267,10 +2268,10 @@
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
       <c r="L12" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="M12" s="3" t="s">
         <v>124</v>
-      </c>
-      <c r="M12" s="3" t="s">
-        <v>123</v>
       </c>
       <c r="N12" s="3" t="s">
         <v>115</v>
@@ -2323,10 +2324,10 @@
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
       <c r="L13" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="M13" s="3" t="s">
         <v>124</v>
-      </c>
-      <c r="M13" s="3" t="s">
-        <v>123</v>
       </c>
       <c r="N13" s="3" t="s">
         <v>112</v>
@@ -2379,10 +2380,10 @@
         <v>108</v>
       </c>
       <c r="L14" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="M14" s="3" t="s">
         <v>88</v>
-      </c>
-      <c r="M14" s="3" t="s">
-        <v>111</v>
       </c>
       <c r="N14" s="3" t="s">
         <v>111</v>
@@ -2435,10 +2436,10 @@
         <v>108</v>
       </c>
       <c r="L15" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="M15" s="3" t="s">
         <v>88</v>
-      </c>
-      <c r="M15" s="3" t="s">
-        <v>112</v>
       </c>
       <c r="N15" s="3" t="s">
         <v>116</v>
@@ -2489,10 +2490,10 @@
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
       <c r="L16" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="M16" s="3" t="s">
         <v>124</v>
-      </c>
-      <c r="M16" s="3" t="s">
-        <v>123</v>
       </c>
       <c r="N16" s="3" t="s">
         <v>117</v>
@@ -2543,10 +2544,10 @@
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
       <c r="L17" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="M17" s="3" t="s">
         <v>124</v>
-      </c>
-      <c r="M17" s="3" t="s">
-        <v>123</v>
       </c>
       <c r="N17" s="3" t="s">
         <v>118</v>
@@ -2597,10 +2598,10 @@
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
       <c r="L18" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="M18" s="3" t="s">
         <v>124</v>
-      </c>
-      <c r="M18" s="3" t="s">
-        <v>123</v>
       </c>
       <c r="N18" s="3" t="s">
         <v>112</v>
@@ -2651,10 +2652,10 @@
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
       <c r="L19" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="M19" s="3" t="s">
         <v>124</v>
-      </c>
-      <c r="M19" s="3" t="s">
-        <v>123</v>
       </c>
       <c r="N19" s="3" t="s">
         <v>112</v>
@@ -2705,10 +2706,10 @@
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
       <c r="L20" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="M20" s="3" t="s">
         <v>124</v>
-      </c>
-      <c r="M20" s="3" t="s">
-        <v>123</v>
       </c>
       <c r="N20" s="3" t="s">
         <v>119</v>
@@ -2759,10 +2760,10 @@
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
       <c r="L21" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="M21" s="3" t="s">
         <v>124</v>
-      </c>
-      <c r="M21" s="3" t="s">
-        <v>123</v>
       </c>
       <c r="N21" s="3" t="s">
         <v>120</v>
@@ -2813,10 +2814,10 @@
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
       <c r="L22" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="M22" s="3" t="s">
         <v>125</v>
-      </c>
-      <c r="M22" s="3" t="s">
-        <v>123</v>
       </c>
       <c r="N22" s="3" t="s">
         <v>114</v>
@@ -2867,10 +2868,10 @@
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
       <c r="L23" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="M23" s="3" t="s">
         <v>125</v>
-      </c>
-      <c r="M23" s="3" t="s">
-        <v>123</v>
       </c>
       <c r="N23" s="3" t="s">
         <v>113</v>
@@ -2923,10 +2924,10 @@
         <v>109</v>
       </c>
       <c r="L24" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="M24" s="3" t="s">
         <v>125</v>
-      </c>
-      <c r="M24" s="3" t="s">
-        <v>113</v>
       </c>
       <c r="N24" s="3" t="s">
         <v>113</v>
@@ -2977,10 +2978,10 @@
       <c r="J25" s="3"/>
       <c r="K25" s="3"/>
       <c r="L25" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="M25" s="3" t="s">
         <v>106</v>
-      </c>
-      <c r="M25" s="3" t="s">
-        <v>123</v>
       </c>
       <c r="N25" s="3" t="s">
         <v>112</v>
@@ -3033,10 +3034,10 @@
         <v>108</v>
       </c>
       <c r="L26" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="M26" s="3" t="s">
         <v>106</v>
-      </c>
-      <c r="M26" s="3" t="s">
-        <v>111</v>
       </c>
       <c r="N26" s="3" t="s">
         <v>112</v>
@@ -3087,10 +3088,10 @@
       <c r="J27" s="3"/>
       <c r="K27" s="3"/>
       <c r="L27" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="M27" s="3" t="s">
         <v>88</v>
-      </c>
-      <c r="M27" s="3" t="s">
-        <v>123</v>
       </c>
       <c r="N27" s="3" t="s">
         <v>121</v>
@@ -3141,10 +3142,10 @@
       <c r="J28" s="3"/>
       <c r="K28" s="3"/>
       <c r="L28" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="M28" s="3" t="s">
         <v>124</v>
-      </c>
-      <c r="M28" s="3" t="s">
-        <v>123</v>
       </c>
       <c r="N28" s="3" t="s">
         <v>120</v>
@@ -3195,10 +3196,10 @@
       <c r="J29" s="3"/>
       <c r="K29" s="3"/>
       <c r="L29" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="M29" s="3" t="s">
         <v>127</v>
-      </c>
-      <c r="M29" s="3" t="s">
-        <v>123</v>
       </c>
       <c r="N29" s="3" t="s">
         <v>112</v>
@@ -3249,10 +3250,10 @@
       <c r="J30" s="3"/>
       <c r="K30" s="3"/>
       <c r="L30" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="M30" s="3" t="s">
         <v>124</v>
-      </c>
-      <c r="M30" s="3" t="s">
-        <v>123</v>
       </c>
       <c r="N30" s="3" t="s">
         <v>111</v>
@@ -3303,10 +3304,10 @@
       <c r="J31" s="3"/>
       <c r="K31" s="3"/>
       <c r="L31" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="M31" s="3" t="s">
         <v>124</v>
-      </c>
-      <c r="M31" s="3" t="s">
-        <v>123</v>
       </c>
       <c r="N31" s="3" t="s">
         <v>122</v>
@@ -3357,10 +3358,10 @@
       <c r="J32" s="3"/>
       <c r="K32" s="3"/>
       <c r="L32" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="M32" s="3" t="s">
         <v>106</v>
-      </c>
-      <c r="M32" s="3" t="s">
-        <v>123</v>
       </c>
       <c r="N32" s="3" t="s">
         <v>120</v>
@@ -3415,10 +3416,10 @@
         <v>108</v>
       </c>
       <c r="L33" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="M33" s="3" t="s">
         <v>106</v>
-      </c>
-      <c r="M33" s="3" t="s">
-        <v>111</v>
       </c>
       <c r="N33" s="3" t="s">
         <v>112</v>

</xml_diff>

<commit_message>
New edits to new scraping data
</commit_message>
<xml_diff>
--- a/analyses/scrapeUSDAseedmanual/scraping/usdaDataScraping_CRD.xlsx
+++ b/analyses/scrapeUSDAseedmanual/scraping/usdaDataScraping_CRD.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christophe_rouleau-desrochers/github/egret/analyses/scrapeUSDAseedmanual/scraping/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PhD\Project\egret\analyses\scrapeUSDAseedmanual\scraping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8165CA8D-1D56-6D41-9812-B527799553BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC624A39-11F7-4944-93CB-9A9997919DF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-30" yWindow="5600" windowWidth="19270" windowHeight="5940" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Meta" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="215">
   <si>
     <t>pdf_page_number</t>
   </si>
@@ -441,9 +441,6 @@
     <t>4.5</t>
   </si>
   <si>
-    <t>20 and 3</t>
-  </si>
-  <si>
     <t>4.4</t>
   </si>
   <si>
@@ -707,6 +704,9 @@
   </si>
   <si>
     <t>prechilling given in text, no details on temperature</t>
+  </si>
+  <si>
+    <t>germ_rate_days</t>
   </si>
 </sst>
 </file>
@@ -717,13 +717,13 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -898,29 +898,29 @@
     <tableColumn id="7" xr3:uid="{7657C123-FA50-ED46-A76A-26AE17978143}" name="pregermination_treatment_time_minutes" dataDxfId="25"/>
     <tableColumn id="8" xr3:uid="{25D42B2B-7F05-4140-A3C6-F8B396550CAB}" name="pregermination_treatment_hot_water_soak_C" dataDxfId="24"/>
     <tableColumn id="9" xr3:uid="{55A4F340-7B6D-7943-8B39-CFAE9E6FE33F}" name="pretreatment" dataDxfId="23"/>
-    <tableColumn id="10" xr3:uid="{4A6EEDC6-97D1-5C4D-8AA2-6F5DFBF4D1C4}" name="stratification_temp_C" dataDxfId="22"/>
-    <tableColumn id="33" xr3:uid="{1210F0BD-23B5-9140-8426-31FF90F8FB3C}" name="warm_stratification_temp_C" dataDxfId="3"/>
-    <tableColumn id="36" xr3:uid="{E51E641D-9B06-5E4C-9658-7002B1B1CEF1}" name="warm_stratification_days" dataDxfId="1"/>
-    <tableColumn id="35" xr3:uid="{FD04900B-878E-AC42-911D-9C9BE08CE010}" name="cold_stratification_temp_C" dataDxfId="2"/>
-    <tableColumn id="34" xr3:uid="{3E825D95-CDE2-874E-89AF-5DD665872E8B}" name="cold_stratification_days" dataDxfId="0"/>
-    <tableColumn id="13" xr3:uid="{FBA71BC1-6F33-B742-9505-31E5F69BC022}" name="dailyl_light_hours" dataDxfId="21"/>
-    <tableColumn id="14" xr3:uid="{B60543C3-E2EE-A64E-A396-1C242453800C}" name="day_temp_celsius" dataDxfId="20"/>
-    <tableColumn id="15" xr3:uid="{A98F0563-6BD3-C049-89CC-CCFA69D88415}" name="night_temp_celsius" dataDxfId="19"/>
-    <tableColumn id="16" xr3:uid="{441701F9-64D9-6C4C-98DD-50E953D9AE81}" name="temp_unspecified_time_of_day_celsius" dataDxfId="18"/>
-    <tableColumn id="17" xr3:uid="{8E32E59C-2511-5E47-B942-01EF1C2F823C}" name="test_duration_in_days" dataDxfId="17"/>
-    <tableColumn id="18" xr3:uid="{427BB247-5A32-DE42-AC51-6837CDABE181}" name="germination_time_days" dataDxfId="16"/>
-    <tableColumn id="19" xr3:uid="{35DE5AFC-901F-3445-96DA-507E967B4ECB}" name="total_germination_percent" dataDxfId="15"/>
-    <tableColumn id="20" xr3:uid="{BC769C61-E4F8-114A-B837-872ED1FFEAAC}" name="avg_germination_percent" dataDxfId="14"/>
-    <tableColumn id="21" xr3:uid="{093E7249-8AC3-8044-8840-C1350D4C13FA}" name="samples" dataDxfId="13"/>
-    <tableColumn id="22" xr3:uid="{4AAA545E-A06B-5A49-A9C2-811A91D56309}" name="germination_rate" dataDxfId="12"/>
-    <tableColumn id="23" xr3:uid="{0E3380FC-04AB-B648-BA64-33C0172712E8}" name="avg_germinative_energy_percent" dataDxfId="11"/>
-    <tableColumn id="24" xr3:uid="{BB029E85-4EEF-7541-A8A6-B78FC45AA990}" name="germinative_energy_percent" dataDxfId="10"/>
-    <tableColumn id="25" xr3:uid="{D9A90743-B6FB-BA4B-951F-4B5A9FC761BA}" name="avg_germinative_capacity" dataDxfId="9"/>
-    <tableColumn id="26" xr3:uid="{5AE4612B-E138-4D40-8419-CC14A92B62CD}" name="germinative_capacity" dataDxfId="8"/>
-    <tableColumn id="27" xr3:uid="{5BE09F3B-7D66-884A-B192-CEE49F2B845E}" name="percent_germination_15degC_incubated" dataDxfId="7"/>
-    <tableColumn id="28" xr3:uid="{6061511F-2CE6-FF4C-BA21-079020EC6884}" name="percent_germination_20degC_incubated" dataDxfId="6"/>
-    <tableColumn id="29" xr3:uid="{B17A6158-E57A-8B49-B7C6-A792A8BB3857}" name="50%_germ" dataDxfId="5"/>
-    <tableColumn id="30" xr3:uid="{C6852079-746D-E843-96F0-451DDB3F34C3}" name="Notes" dataDxfId="4"/>
+    <tableColumn id="33" xr3:uid="{1210F0BD-23B5-9140-8426-31FF90F8FB3C}" name="warm_stratification_temp_C" dataDxfId="22"/>
+    <tableColumn id="36" xr3:uid="{E51E641D-9B06-5E4C-9658-7002B1B1CEF1}" name="warm_stratification_days" dataDxfId="21"/>
+    <tableColumn id="35" xr3:uid="{FD04900B-878E-AC42-911D-9C9BE08CE010}" name="cold_stratification_temp_C" dataDxfId="20"/>
+    <tableColumn id="34" xr3:uid="{3E825D95-CDE2-874E-89AF-5DD665872E8B}" name="cold_stratification_days" dataDxfId="19"/>
+    <tableColumn id="13" xr3:uid="{FBA71BC1-6F33-B742-9505-31E5F69BC022}" name="dailyl_light_hours" dataDxfId="18"/>
+    <tableColumn id="14" xr3:uid="{B60543C3-E2EE-A64E-A396-1C242453800C}" name="day_temp_celsius" dataDxfId="17"/>
+    <tableColumn id="15" xr3:uid="{A98F0563-6BD3-C049-89CC-CCFA69D88415}" name="night_temp_celsius" dataDxfId="16"/>
+    <tableColumn id="16" xr3:uid="{441701F9-64D9-6C4C-98DD-50E953D9AE81}" name="temp_unspecified_time_of_day_celsius" dataDxfId="15"/>
+    <tableColumn id="17" xr3:uid="{8E32E59C-2511-5E47-B942-01EF1C2F823C}" name="test_duration_in_days" dataDxfId="14"/>
+    <tableColumn id="18" xr3:uid="{427BB247-5A32-DE42-AC51-6837CDABE181}" name="germination_time_days" dataDxfId="13"/>
+    <tableColumn id="19" xr3:uid="{35DE5AFC-901F-3445-96DA-507E967B4ECB}" name="total_germination_percent" dataDxfId="12"/>
+    <tableColumn id="20" xr3:uid="{BC769C61-E4F8-114A-B837-872ED1FFEAAC}" name="avg_germination_percent" dataDxfId="11"/>
+    <tableColumn id="21" xr3:uid="{093E7249-8AC3-8044-8840-C1350D4C13FA}" name="samples" dataDxfId="10"/>
+    <tableColumn id="22" xr3:uid="{4AAA545E-A06B-5A49-A9C2-811A91D56309}" name="germination_rate" dataDxfId="9"/>
+    <tableColumn id="23" xr3:uid="{0E3380FC-04AB-B648-BA64-33C0172712E8}" name="avg_germinative_energy_percent" dataDxfId="8"/>
+    <tableColumn id="24" xr3:uid="{BB029E85-4EEF-7541-A8A6-B78FC45AA990}" name="germinative_energy_percent" dataDxfId="7"/>
+    <tableColumn id="25" xr3:uid="{D9A90743-B6FB-BA4B-951F-4B5A9FC761BA}" name="avg_germinative_capacity" dataDxfId="6"/>
+    <tableColumn id="26" xr3:uid="{5AE4612B-E138-4D40-8419-CC14A92B62CD}" name="germinative_capacity" dataDxfId="5"/>
+    <tableColumn id="27" xr3:uid="{5BE09F3B-7D66-884A-B192-CEE49F2B845E}" name="percent_germination_15degC_incubated" dataDxfId="4"/>
+    <tableColumn id="28" xr3:uid="{6061511F-2CE6-FF4C-BA21-079020EC6884}" name="percent_germination_20degC_incubated" dataDxfId="3"/>
+    <tableColumn id="10" xr3:uid="{89D5B3B5-8BC9-4BAA-8D45-AB924C4812E9}" name="germ_rate_days" dataDxfId="0"/>
+    <tableColumn id="29" xr3:uid="{B17A6158-E57A-8B49-B7C6-A792A8BB3857}" name="50%_germ" dataDxfId="2"/>
+    <tableColumn id="30" xr3:uid="{C6852079-746D-E843-96F0-451DDB3F34C3}" name="Notes" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1195,7 +1195,7 @@
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="41.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
@@ -1209,7 +1209,7 @@
     <col min="10" max="10" width="41.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1251,7 +1251,7 @@
       <c r="AI1" s="1"/>
       <c r="AJ1" s="1"/>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1259,7 +1259,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1267,7 +1267,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -1275,7 +1275,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1283,7 +1283,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1291,7 +1291,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -1299,7 +1299,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -1307,7 +1307,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -1315,7 +1315,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -1323,7 +1323,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -1331,7 +1331,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -1339,7 +1339,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -1347,7 +1347,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
@@ -1355,7 +1355,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -1363,7 +1363,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -1371,7 +1371,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
@@ -1379,7 +1379,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>66</v>
       </c>
@@ -1387,7 +1387,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>65</v>
       </c>
@@ -1395,7 +1395,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>64</v>
       </c>
@@ -1403,7 +1403,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
@@ -1411,7 +1411,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
@@ -1419,7 +1419,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
@@ -1427,7 +1427,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
@@ -1435,7 +1435,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
@@ -1443,7 +1443,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
@@ -1451,7 +1451,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>26</v>
       </c>
@@ -1459,7 +1459,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>27</v>
       </c>
@@ -1467,7 +1467,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>52</v>
       </c>
@@ -1475,7 +1475,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>53</v>
       </c>
@@ -1483,22 +1483,22 @@
         <v>58</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>63</v>
       </c>
@@ -1514,11 +1514,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4AC4DDB-17EE-463A-9304-F699F6DBC2E2}">
   <dimension ref="A1:AF47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T14" zoomScale="125" workbookViewId="0">
-      <selection activeCell="AF8" sqref="AF8"/>
+    <sheetView tabSelected="1" topLeftCell="AB1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="AG2" sqref="AG2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.83203125" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
@@ -1528,28 +1528,28 @@
     <col min="7" max="7" width="33.6640625" customWidth="1"/>
     <col min="8" max="8" width="37.1640625" customWidth="1"/>
     <col min="9" max="9" width="12" customWidth="1"/>
-    <col min="10" max="10" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="14" width="20.5" customWidth="1"/>
-    <col min="15" max="15" width="15.5" customWidth="1"/>
-    <col min="16" max="16" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="34.6640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="20.83203125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="22" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="25" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="30" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="26.5" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="29" max="30" width="36.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="13" width="20.5" customWidth="1"/>
+    <col min="14" max="14" width="15.5" customWidth="1"/>
+    <col min="15" max="15" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="34.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="22" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="25" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="30" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="26.5" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="28" max="29" width="36.1640625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="36.1640625" customWidth="1"/>
     <col min="31" max="31" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="8.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1578,67 +1578,67 @@
         <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>9</v>
+        <v>210</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>211</v>
+        <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>10</v>
+        <v>212</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>213</v>
+        <v>11</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>27</v>
+        <v>214</v>
       </c>
       <c r="AE1" s="2" t="s">
         <v>52</v>
@@ -1647,7 +1647,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>703</v>
       </c>
@@ -1672,42 +1672,42 @@
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
+      <c r="O2" s="3" t="s">
+        <v>80</v>
+      </c>
       <c r="P2" s="3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="S2" s="3"/>
+        <v>76</v>
+      </c>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3" t="s">
+        <v>206</v>
+      </c>
       <c r="T2" s="3" t="s">
-        <v>207</v>
+        <v>76</v>
       </c>
       <c r="U2" s="3" t="s">
         <v>76</v>
       </c>
       <c r="V2" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="W2" s="3" t="s">
         <v>88</v>
       </c>
+      <c r="W2" s="3"/>
       <c r="X2" s="3"/>
       <c r="Y2" s="3"/>
-      <c r="Z2" s="3"/>
-      <c r="AA2" s="3" t="s">
-        <v>203</v>
-      </c>
+      <c r="Z2" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="AA2" s="3"/>
       <c r="AB2" s="3"/>
       <c r="AC2" s="3"/>
       <c r="AD2" s="3"/>
       <c r="AE2" s="3"/>
       <c r="AF2" s="3"/>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>703</v>
       </c>
@@ -1732,42 +1732,42 @@
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
+      <c r="O3" s="3">
+        <v>30</v>
+      </c>
       <c r="P3" s="3">
-        <v>30</v>
-      </c>
-      <c r="Q3" s="3">
         <v>20</v>
       </c>
-      <c r="R3" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="S3" s="3"/>
+      <c r="Q3" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="R3" s="3"/>
+      <c r="S3" s="3" t="s">
+        <v>207</v>
+      </c>
       <c r="T3" s="3" t="s">
-        <v>208</v>
+        <v>76</v>
       </c>
       <c r="U3" s="3" t="s">
         <v>76</v>
       </c>
       <c r="V3" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="W3" s="3" t="s">
         <v>89</v>
       </c>
+      <c r="W3" s="3"/>
       <c r="X3" s="3"/>
       <c r="Y3" s="3"/>
-      <c r="Z3" s="3"/>
-      <c r="AA3" s="3" t="s">
-        <v>204</v>
-      </c>
+      <c r="Z3" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="AA3" s="3"/>
       <c r="AB3" s="3"/>
       <c r="AC3" s="3"/>
       <c r="AD3" s="3"/>
       <c r="AE3" s="3"/>
       <c r="AF3" s="3"/>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>703</v>
       </c>
@@ -1792,42 +1792,42 @@
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
-      <c r="O4" s="3"/>
+      <c r="O4" s="3">
+        <v>30</v>
+      </c>
       <c r="P4" s="3">
-        <v>30</v>
-      </c>
-      <c r="Q4" s="3">
         <v>20</v>
       </c>
-      <c r="R4" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="S4" s="3"/>
+      <c r="Q4" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3" t="s">
+        <v>208</v>
+      </c>
       <c r="T4" s="3" t="s">
-        <v>209</v>
+        <v>76</v>
       </c>
       <c r="U4" s="3" t="s">
         <v>76</v>
       </c>
       <c r="V4" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="W4" s="3" t="s">
         <v>90</v>
       </c>
+      <c r="W4" s="3"/>
       <c r="X4" s="3"/>
       <c r="Y4" s="3"/>
-      <c r="Z4" s="3"/>
-      <c r="AA4" s="3" t="s">
-        <v>205</v>
-      </c>
+      <c r="Z4" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="AA4" s="3"/>
       <c r="AB4" s="3"/>
       <c r="AC4" s="3"/>
       <c r="AD4" s="3"/>
       <c r="AE4" s="3"/>
       <c r="AF4" s="3"/>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>703</v>
       </c>
@@ -1852,42 +1852,42 @@
       <c r="L5" s="3"/>
       <c r="M5" s="3"/>
       <c r="N5" s="3"/>
-      <c r="O5" s="3"/>
+      <c r="O5" s="3">
+        <v>22</v>
+      </c>
       <c r="P5" s="3">
         <v>22</v>
       </c>
-      <c r="Q5" s="3">
-        <v>22</v>
-      </c>
-      <c r="R5" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="S5" s="3"/>
-      <c r="T5" s="3">
+      <c r="Q5" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="R5" s="3"/>
+      <c r="S5" s="3">
         <v>35</v>
       </c>
+      <c r="T5" s="3" t="s">
+        <v>76</v>
+      </c>
       <c r="U5" s="3" t="s">
         <v>76</v>
       </c>
       <c r="V5" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="W5" s="3" t="s">
         <v>91</v>
       </c>
+      <c r="W5" s="3"/>
       <c r="X5" s="3"/>
       <c r="Y5" s="3"/>
-      <c r="Z5" s="3"/>
-      <c r="AA5" s="3" t="s">
+      <c r="Z5" s="3" t="s">
         <v>82</v>
       </c>
+      <c r="AA5" s="3"/>
       <c r="AB5" s="3"/>
       <c r="AC5" s="3"/>
       <c r="AD5" s="3"/>
       <c r="AE5" s="3"/>
       <c r="AF5" s="3"/>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>703</v>
       </c>
@@ -1912,42 +1912,42 @@
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
       <c r="N6" s="3"/>
-      <c r="O6" s="3"/>
+      <c r="O6" s="3">
+        <v>24</v>
+      </c>
       <c r="P6" s="3">
-        <v>24</v>
-      </c>
-      <c r="Q6" s="3">
         <v>30</v>
       </c>
-      <c r="R6" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="S6" s="3"/>
-      <c r="T6" s="3">
+      <c r="Q6" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3">
         <v>44</v>
       </c>
+      <c r="T6" s="3" t="s">
+        <v>76</v>
+      </c>
       <c r="U6" s="3" t="s">
         <v>76</v>
       </c>
       <c r="V6" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="W6" s="3" t="s">
-        <v>76</v>
-      </c>
+      <c r="W6" s="3"/>
       <c r="X6" s="3"/>
       <c r="Y6" s="3"/>
-      <c r="Z6" s="3"/>
-      <c r="AA6" s="3" t="s">
+      <c r="Z6" s="3" t="s">
         <v>86</v>
       </c>
+      <c r="AA6" s="3"/>
       <c r="AB6" s="3"/>
       <c r="AC6" s="3"/>
       <c r="AD6" s="3"/>
       <c r="AE6" s="3"/>
       <c r="AF6" s="3"/>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>703</v>
       </c>
@@ -1969,53 +1969,51 @@
       <c r="I7" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="J7" s="3" t="s">
-        <v>76</v>
-      </c>
+      <c r="J7" s="3"/>
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="3" t="s">
+      <c r="M7" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="O7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3">
+        <v>18</v>
+      </c>
       <c r="P7" s="3">
         <v>18</v>
       </c>
-      <c r="Q7" s="3">
-        <v>18</v>
-      </c>
-      <c r="R7" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="S7" s="3"/>
-      <c r="T7" s="3">
+      <c r="Q7" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="R7" s="3"/>
+      <c r="S7" s="3">
         <v>33</v>
       </c>
+      <c r="T7" s="3" t="s">
+        <v>76</v>
+      </c>
       <c r="U7" s="3" t="s">
         <v>76</v>
       </c>
       <c r="V7" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="W7" s="3" t="s">
         <v>92</v>
       </c>
+      <c r="W7" s="3"/>
       <c r="X7" s="3"/>
       <c r="Y7" s="3"/>
-      <c r="Z7" s="3"/>
-      <c r="AA7" s="3" t="s">
+      <c r="Z7" s="3" t="s">
         <v>87</v>
       </c>
+      <c r="AA7" s="3"/>
       <c r="AB7" s="3"/>
       <c r="AC7" s="3"/>
       <c r="AD7" s="3"/>
       <c r="AE7" s="3"/>
       <c r="AF7" s="3" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.2">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="8" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>703</v>
       </c>
@@ -2040,42 +2038,42 @@
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
       <c r="N8" s="3"/>
-      <c r="O8" s="3"/>
+      <c r="O8" s="3">
+        <v>30</v>
+      </c>
       <c r="P8" s="3">
-        <v>30</v>
-      </c>
-      <c r="Q8" s="3">
         <v>20</v>
       </c>
-      <c r="R8" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="S8" s="3"/>
+      <c r="Q8" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="R8" s="3"/>
+      <c r="S8" s="3" t="s">
+        <v>209</v>
+      </c>
       <c r="T8" s="3" t="s">
-        <v>210</v>
+        <v>76</v>
       </c>
       <c r="U8" s="3" t="s">
         <v>76</v>
       </c>
       <c r="V8" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="W8" s="3" t="s">
         <v>88</v>
       </c>
+      <c r="W8" s="3"/>
       <c r="X8" s="3"/>
       <c r="Y8" s="3"/>
-      <c r="Z8" s="3"/>
-      <c r="AA8" s="3" t="s">
-        <v>206</v>
-      </c>
+      <c r="Z8" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="AA8" s="3"/>
       <c r="AB8" s="3"/>
       <c r="AC8" s="3"/>
       <c r="AD8" s="3"/>
       <c r="AE8" s="3"/>
       <c r="AF8" s="3"/>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>105</v>
       </c>
@@ -2093,30 +2091,30 @@
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
       <c r="I9" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
+      <c r="K9" s="3" t="s">
+        <v>123</v>
+      </c>
       <c r="L9" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="N9" s="3" t="s">
         <v>114</v>
       </c>
+      <c r="N9" s="3"/>
       <c r="O9" s="3"/>
       <c r="P9" s="3"/>
-      <c r="Q9" s="3"/>
-      <c r="R9" s="3" t="s">
+      <c r="Q9" s="3" t="s">
         <v>124</v>
       </c>
+      <c r="R9" s="3"/>
       <c r="S9" s="3"/>
-      <c r="T9" s="3"/>
-      <c r="U9" s="3" t="s">
+      <c r="T9" s="3" t="s">
         <v>83</v>
       </c>
+      <c r="U9" s="3"/>
       <c r="V9" s="3"/>
       <c r="W9" s="3"/>
       <c r="X9" s="3"/>
@@ -2128,10 +2126,10 @@
       <c r="AD9" s="3"/>
       <c r="AE9" s="3"/>
       <c r="AF9" s="3" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.2">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="10" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>105</v>
       </c>
@@ -2149,32 +2147,32 @@
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
       <c r="I10" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="J10" s="3"/>
+        <v>151</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>211</v>
+      </c>
       <c r="K10" s="3" t="s">
-        <v>212</v>
+        <v>110</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>110</v>
+        <v>124</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="N10" s="3" t="s">
         <v>112</v>
       </c>
+      <c r="N10" s="3"/>
       <c r="O10" s="3"/>
       <c r="P10" s="3"/>
-      <c r="Q10" s="3"/>
-      <c r="R10" s="4" t="s">
-        <v>146</v>
-      </c>
+      <c r="Q10" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="R10" s="3"/>
       <c r="S10" s="3"/>
-      <c r="T10" s="3"/>
-      <c r="U10" s="3" t="s">
+      <c r="T10" s="3" t="s">
         <v>112</v>
       </c>
+      <c r="U10" s="3"/>
       <c r="V10" s="3"/>
       <c r="W10" s="3"/>
       <c r="X10" s="3"/>
@@ -2186,10 +2184,10 @@
       <c r="AD10" s="3"/>
       <c r="AE10" s="3"/>
       <c r="AF10" s="3" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.2">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="11" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>105</v>
       </c>
@@ -2207,30 +2205,30 @@
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
       <c r="I11" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
+      <c r="K11" s="3" t="s">
+        <v>123</v>
+      </c>
       <c r="L11" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="M11" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="N11" s="3" t="s">
         <v>112</v>
       </c>
+      <c r="N11" s="3"/>
       <c r="O11" s="3"/>
       <c r="P11" s="3"/>
-      <c r="Q11" s="3"/>
-      <c r="R11" s="3" t="s">
-        <v>147</v>
-      </c>
+      <c r="Q11" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="R11" s="3"/>
       <c r="S11" s="3"/>
-      <c r="T11" s="3"/>
-      <c r="U11" s="3" t="s">
-        <v>128</v>
-      </c>
+      <c r="T11" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="U11" s="3"/>
       <c r="V11" s="3"/>
       <c r="W11" s="3"/>
       <c r="X11" s="3"/>
@@ -2242,10 +2240,10 @@
       <c r="AD11" s="3"/>
       <c r="AE11" s="3"/>
       <c r="AF11" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.2">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="12" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>105</v>
       </c>
@@ -2263,30 +2261,30 @@
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
       <c r="I12" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
+      <c r="K12" s="3" t="s">
+        <v>123</v>
+      </c>
       <c r="L12" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="M12" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="N12" s="3" t="s">
         <v>115</v>
       </c>
+      <c r="N12" s="3"/>
       <c r="O12" s="3"/>
       <c r="P12" s="3"/>
-      <c r="Q12" s="3"/>
-      <c r="R12" s="3" t="s">
-        <v>147</v>
-      </c>
+      <c r="Q12" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="R12" s="3"/>
       <c r="S12" s="3"/>
-      <c r="T12" s="3"/>
-      <c r="U12" s="3" t="s">
-        <v>129</v>
-      </c>
+      <c r="T12" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="U12" s="3"/>
       <c r="V12" s="3"/>
       <c r="W12" s="3"/>
       <c r="X12" s="3"/>
@@ -2298,10 +2296,10 @@
       <c r="AD12" s="3"/>
       <c r="AE12" s="3"/>
       <c r="AF12" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.2">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="13" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>105</v>
       </c>
@@ -2319,30 +2317,30 @@
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
       <c r="I13" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
+      <c r="K13" s="3" t="s">
+        <v>123</v>
+      </c>
       <c r="L13" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="M13" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="N13" s="3" t="s">
         <v>112</v>
       </c>
+      <c r="N13" s="3"/>
       <c r="O13" s="3"/>
       <c r="P13" s="3"/>
-      <c r="Q13" s="3"/>
-      <c r="R13" s="3" t="s">
-        <v>76</v>
-      </c>
+      <c r="Q13" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="R13" s="3"/>
       <c r="S13" s="3"/>
-      <c r="T13" s="3"/>
-      <c r="U13" s="3" t="s">
-        <v>130</v>
-      </c>
+      <c r="T13" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="U13" s="3"/>
       <c r="V13" s="3"/>
       <c r="W13" s="3"/>
       <c r="X13" s="3"/>
@@ -2355,7 +2353,7 @@
       <c r="AE13" s="3"/>
       <c r="AF13" s="3"/>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>105</v>
       </c>
@@ -2373,32 +2371,32 @@
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
       <c r="I14" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="J14" s="3"/>
+        <v>151</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>108</v>
+      </c>
       <c r="K14" s="3" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="L14" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="M14" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="M14" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="N14" s="3" t="s">
-        <v>111</v>
-      </c>
+      <c r="N14" s="3"/>
       <c r="O14" s="3"/>
       <c r="P14" s="3"/>
-      <c r="Q14" s="3"/>
-      <c r="R14" s="3" t="s">
-        <v>76</v>
-      </c>
+      <c r="Q14" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="R14" s="3"/>
       <c r="S14" s="3"/>
-      <c r="T14" s="3"/>
-      <c r="U14" s="3" t="s">
-        <v>131</v>
-      </c>
+      <c r="T14" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="U14" s="3"/>
       <c r="V14" s="3"/>
       <c r="W14" s="3"/>
       <c r="X14" s="3"/>
@@ -2411,7 +2409,7 @@
       <c r="AE14" s="3"/>
       <c r="AF14" s="3"/>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>105</v>
       </c>
@@ -2429,32 +2427,32 @@
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
       <c r="I15" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="J15" s="3"/>
+        <v>151</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>108</v>
+      </c>
       <c r="K15" s="3" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="L15" s="3" t="s">
-        <v>112</v>
+        <v>88</v>
       </c>
       <c r="M15" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="N15" s="3" t="s">
         <v>116</v>
       </c>
+      <c r="N15" s="3"/>
       <c r="O15" s="3"/>
       <c r="P15" s="3"/>
-      <c r="Q15" s="3"/>
-      <c r="R15" s="3" t="s">
-        <v>76</v>
-      </c>
+      <c r="Q15" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="R15" s="3"/>
       <c r="S15" s="3"/>
-      <c r="T15" s="3"/>
-      <c r="U15" s="3" t="s">
-        <v>132</v>
-      </c>
+      <c r="T15" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="U15" s="3"/>
       <c r="V15" s="3"/>
       <c r="W15" s="3"/>
       <c r="X15" s="3"/>
@@ -2467,7 +2465,7 @@
       <c r="AE15" s="3"/>
       <c r="AF15" s="3"/>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>105</v>
       </c>
@@ -2485,30 +2483,30 @@
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
       <c r="I16" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
+      <c r="K16" s="3" t="s">
+        <v>123</v>
+      </c>
       <c r="L16" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="M16" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="N16" s="3" t="s">
         <v>117</v>
       </c>
+      <c r="N16" s="3"/>
       <c r="O16" s="3"/>
       <c r="P16" s="3"/>
-      <c r="Q16" s="3"/>
-      <c r="R16" s="3" t="s">
+      <c r="Q16" s="3" t="s">
         <v>124</v>
       </c>
+      <c r="R16" s="3"/>
       <c r="S16" s="3"/>
-      <c r="T16" s="3"/>
-      <c r="U16" s="3" t="s">
-        <v>133</v>
-      </c>
+      <c r="T16" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="U16" s="3"/>
       <c r="V16" s="3"/>
       <c r="W16" s="3"/>
       <c r="X16" s="3"/>
@@ -2521,7 +2519,7 @@
       <c r="AE16" s="3"/>
       <c r="AF16" s="3"/>
     </row>
-    <row r="17" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>105</v>
       </c>
@@ -2539,30 +2537,30 @@
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
       <c r="I17" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
+      <c r="K17" s="3" t="s">
+        <v>123</v>
+      </c>
       <c r="L17" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="M17" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="N17" s="3" t="s">
         <v>118</v>
       </c>
+      <c r="N17" s="3"/>
       <c r="O17" s="3"/>
       <c r="P17" s="3"/>
-      <c r="Q17" s="3"/>
-      <c r="R17" s="3" t="s">
+      <c r="Q17" s="3" t="s">
         <v>124</v>
       </c>
+      <c r="R17" s="3"/>
       <c r="S17" s="3"/>
-      <c r="T17" s="3"/>
-      <c r="U17" s="3" t="s">
-        <v>134</v>
-      </c>
+      <c r="T17" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="U17" s="3"/>
       <c r="V17" s="3"/>
       <c r="W17" s="3"/>
       <c r="X17" s="3"/>
@@ -2575,7 +2573,7 @@
       <c r="AE17" s="3"/>
       <c r="AF17" s="3"/>
     </row>
-    <row r="18" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>105</v>
       </c>
@@ -2593,30 +2591,30 @@
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
       <c r="I18" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
+      <c r="K18" s="3" t="s">
+        <v>123</v>
+      </c>
       <c r="L18" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="M18" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="N18" s="3" t="s">
         <v>112</v>
       </c>
+      <c r="N18" s="3"/>
       <c r="O18" s="3"/>
       <c r="P18" s="3"/>
-      <c r="Q18" s="3"/>
-      <c r="R18" s="3" t="s">
-        <v>76</v>
-      </c>
+      <c r="Q18" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="R18" s="3"/>
       <c r="S18" s="3"/>
-      <c r="T18" s="3"/>
-      <c r="U18" s="3" t="s">
-        <v>135</v>
-      </c>
+      <c r="T18" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="U18" s="3"/>
       <c r="V18" s="3"/>
       <c r="W18" s="3"/>
       <c r="X18" s="3"/>
@@ -2629,7 +2627,7 @@
       <c r="AE18" s="3"/>
       <c r="AF18" s="3"/>
     </row>
-    <row r="19" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>105</v>
       </c>
@@ -2647,30 +2645,30 @@
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
       <c r="I19" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
+      <c r="K19" s="3" t="s">
+        <v>123</v>
+      </c>
       <c r="L19" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="M19" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="N19" s="3" t="s">
         <v>112</v>
       </c>
+      <c r="N19" s="3"/>
       <c r="O19" s="3"/>
       <c r="P19" s="3"/>
-      <c r="Q19" s="3"/>
-      <c r="R19" s="3" t="s">
-        <v>148</v>
-      </c>
+      <c r="Q19" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="R19" s="3"/>
       <c r="S19" s="3"/>
-      <c r="T19" s="3"/>
-      <c r="U19" s="3" t="s">
+      <c r="T19" s="3" t="s">
         <v>122</v>
       </c>
+      <c r="U19" s="3"/>
       <c r="V19" s="3"/>
       <c r="W19" s="3"/>
       <c r="X19" s="3"/>
@@ -2683,7 +2681,7 @@
       <c r="AE19" s="3"/>
       <c r="AF19" s="3"/>
     </row>
-    <row r="20" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>105</v>
       </c>
@@ -2701,30 +2699,30 @@
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
       <c r="I20" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J20" s="3"/>
-      <c r="K20" s="3"/>
+      <c r="K20" s="3" t="s">
+        <v>123</v>
+      </c>
       <c r="L20" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="M20" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="N20" s="3" t="s">
         <v>119</v>
       </c>
+      <c r="N20" s="3"/>
       <c r="O20" s="3"/>
       <c r="P20" s="3"/>
-      <c r="Q20" s="3"/>
-      <c r="R20" s="3" t="s">
-        <v>148</v>
-      </c>
+      <c r="Q20" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="R20" s="3"/>
       <c r="S20" s="3"/>
-      <c r="T20" s="3"/>
-      <c r="U20" s="3" t="s">
+      <c r="T20" s="3" t="s">
         <v>111</v>
       </c>
+      <c r="U20" s="3"/>
       <c r="V20" s="3"/>
       <c r="W20" s="3"/>
       <c r="X20" s="3"/>
@@ -2737,7 +2735,7 @@
       <c r="AE20" s="3"/>
       <c r="AF20" s="3"/>
     </row>
-    <row r="21" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>105</v>
       </c>
@@ -2755,30 +2753,30 @@
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
       <c r="I21" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J21" s="3"/>
-      <c r="K21" s="3"/>
+      <c r="K21" s="3" t="s">
+        <v>123</v>
+      </c>
       <c r="L21" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="M21" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="N21" s="3" t="s">
         <v>120</v>
       </c>
+      <c r="N21" s="3"/>
       <c r="O21" s="3"/>
       <c r="P21" s="3"/>
-      <c r="Q21" s="3"/>
-      <c r="R21" s="3" t="s">
+      <c r="Q21" s="3" t="s">
         <v>124</v>
       </c>
+      <c r="R21" s="3"/>
       <c r="S21" s="3"/>
-      <c r="T21" s="3"/>
-      <c r="U21" s="3" t="s">
-        <v>136</v>
-      </c>
+      <c r="T21" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="U21" s="3"/>
       <c r="V21" s="3"/>
       <c r="W21" s="3"/>
       <c r="X21" s="3"/>
@@ -2791,7 +2789,7 @@
       <c r="AE21" s="3"/>
       <c r="AF21" s="3"/>
     </row>
-    <row r="22" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>105</v>
       </c>
@@ -2809,30 +2807,30 @@
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
       <c r="I22" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J22" s="3"/>
-      <c r="K22" s="3"/>
+      <c r="K22" s="3" t="s">
+        <v>123</v>
+      </c>
       <c r="L22" s="3" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="M22" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="N22" s="3" t="s">
         <v>114</v>
       </c>
+      <c r="N22" s="3"/>
       <c r="O22" s="3"/>
       <c r="P22" s="3"/>
-      <c r="Q22" s="3"/>
-      <c r="R22" s="3" t="s">
+      <c r="Q22" s="3" t="s">
         <v>125</v>
       </c>
+      <c r="R22" s="3"/>
       <c r="S22" s="3"/>
-      <c r="T22" s="3"/>
-      <c r="U22" s="3" t="s">
-        <v>137</v>
-      </c>
+      <c r="T22" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="U22" s="3"/>
       <c r="V22" s="3"/>
       <c r="W22" s="3"/>
       <c r="X22" s="3"/>
@@ -2845,7 +2843,7 @@
       <c r="AE22" s="3"/>
       <c r="AF22" s="3"/>
     </row>
-    <row r="23" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>105</v>
       </c>
@@ -2863,30 +2861,30 @@
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
       <c r="I23" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J23" s="3"/>
-      <c r="K23" s="3"/>
+      <c r="K23" s="3" t="s">
+        <v>123</v>
+      </c>
       <c r="L23" s="3" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="M23" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="N23" s="3" t="s">
         <v>113</v>
       </c>
+      <c r="N23" s="3"/>
       <c r="O23" s="3"/>
       <c r="P23" s="3"/>
-      <c r="Q23" s="3"/>
-      <c r="R23" s="3" t="s">
+      <c r="Q23" s="3" t="s">
         <v>109</v>
       </c>
+      <c r="R23" s="3"/>
       <c r="S23" s="3"/>
-      <c r="T23" s="3"/>
-      <c r="U23" s="3" t="s">
-        <v>138</v>
-      </c>
+      <c r="T23" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="U23" s="3"/>
       <c r="V23" s="3"/>
       <c r="W23" s="3"/>
       <c r="X23" s="3"/>
@@ -2899,7 +2897,7 @@
       <c r="AE23" s="3"/>
       <c r="AF23" s="3"/>
     </row>
-    <row r="24" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>105</v>
       </c>
@@ -2917,32 +2915,32 @@
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
       <c r="I24" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="J24" s="3"/>
+        <v>151</v>
+      </c>
+      <c r="J24" s="3" t="s">
+        <v>109</v>
+      </c>
       <c r="K24" s="3" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="L24" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="M24" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="M24" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="N24" s="3" t="s">
-        <v>113</v>
-      </c>
+      <c r="N24" s="3"/>
       <c r="O24" s="3"/>
       <c r="P24" s="3"/>
-      <c r="Q24" s="3"/>
-      <c r="R24" s="3" t="s">
+      <c r="Q24" s="3" t="s">
         <v>109</v>
       </c>
+      <c r="R24" s="3"/>
       <c r="S24" s="3"/>
-      <c r="T24" s="3"/>
-      <c r="U24" s="3" t="s">
-        <v>136</v>
-      </c>
+      <c r="T24" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="U24" s="3"/>
       <c r="V24" s="3"/>
       <c r="W24" s="3"/>
       <c r="X24" s="3"/>
@@ -2955,7 +2953,7 @@
       <c r="AE24" s="3"/>
       <c r="AF24" s="3"/>
     </row>
-    <row r="25" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>105</v>
       </c>
@@ -2973,30 +2971,30 @@
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
       <c r="I25" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J25" s="3"/>
-      <c r="K25" s="3"/>
+      <c r="K25" s="3" t="s">
+        <v>123</v>
+      </c>
       <c r="L25" s="3" t="s">
-        <v>123</v>
+        <v>106</v>
       </c>
       <c r="M25" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="N25" s="3" t="s">
         <v>112</v>
       </c>
+      <c r="N25" s="3"/>
       <c r="O25" s="3"/>
       <c r="P25" s="3"/>
-      <c r="Q25" s="3"/>
-      <c r="R25" s="3" t="s">
-        <v>149</v>
-      </c>
+      <c r="Q25" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="R25" s="3"/>
       <c r="S25" s="3"/>
-      <c r="T25" s="3"/>
-      <c r="U25" s="3" t="s">
-        <v>139</v>
-      </c>
+      <c r="T25" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="U25" s="3"/>
       <c r="V25" s="3"/>
       <c r="W25" s="3"/>
       <c r="X25" s="3"/>
@@ -3009,7 +3007,7 @@
       <c r="AE25" s="3"/>
       <c r="AF25" s="3"/>
     </row>
-    <row r="26" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>105</v>
       </c>
@@ -3027,32 +3025,32 @@
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
       <c r="I26" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="J26" s="3"/>
+        <v>151</v>
+      </c>
+      <c r="J26" s="3" t="s">
+        <v>108</v>
+      </c>
       <c r="K26" s="3" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="L26" s="3" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="M26" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="N26" s="3" t="s">
         <v>112</v>
       </c>
+      <c r="N26" s="3"/>
       <c r="O26" s="3"/>
       <c r="P26" s="3"/>
-      <c r="Q26" s="3"/>
-      <c r="R26" s="3" t="s">
-        <v>149</v>
-      </c>
+      <c r="Q26" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="R26" s="3"/>
       <c r="S26" s="3"/>
-      <c r="T26" s="3"/>
-      <c r="U26" s="3" t="s">
+      <c r="T26" s="3" t="s">
         <v>111</v>
       </c>
+      <c r="U26" s="3"/>
       <c r="V26" s="3"/>
       <c r="W26" s="3"/>
       <c r="X26" s="3"/>
@@ -3065,7 +3063,7 @@
       <c r="AE26" s="3"/>
       <c r="AF26" s="3"/>
     </row>
-    <row r="27" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>105</v>
       </c>
@@ -3083,30 +3081,30 @@
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
       <c r="I27" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J27" s="3"/>
-      <c r="K27" s="3"/>
+      <c r="K27" s="3" t="s">
+        <v>123</v>
+      </c>
       <c r="L27" s="3" t="s">
-        <v>123</v>
+        <v>88</v>
       </c>
       <c r="M27" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="N27" s="3" t="s">
         <v>121</v>
       </c>
+      <c r="N27" s="3"/>
       <c r="O27" s="3"/>
       <c r="P27" s="3"/>
-      <c r="Q27" s="3"/>
-      <c r="R27" s="3" t="s">
+      <c r="Q27" s="3" t="s">
         <v>108</v>
       </c>
+      <c r="R27" s="3"/>
       <c r="S27" s="3"/>
-      <c r="T27" s="3"/>
-      <c r="U27" s="3" t="s">
-        <v>140</v>
-      </c>
+      <c r="T27" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="U27" s="3"/>
       <c r="V27" s="3"/>
       <c r="W27" s="3"/>
       <c r="X27" s="3"/>
@@ -3119,7 +3117,7 @@
       <c r="AE27" s="3"/>
       <c r="AF27" s="3"/>
     </row>
-    <row r="28" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>105</v>
       </c>
@@ -3137,30 +3135,30 @@
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
       <c r="I28" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J28" s="3"/>
-      <c r="K28" s="3"/>
+      <c r="K28" s="3" t="s">
+        <v>123</v>
+      </c>
       <c r="L28" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="M28" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="N28" s="3" t="s">
         <v>120</v>
       </c>
+      <c r="N28" s="3"/>
       <c r="O28" s="3"/>
       <c r="P28" s="3"/>
-      <c r="Q28" s="3"/>
-      <c r="R28" s="3" t="s">
-        <v>148</v>
-      </c>
+      <c r="Q28" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="R28" s="3"/>
       <c r="S28" s="3"/>
-      <c r="T28" s="3"/>
-      <c r="U28" s="3" t="s">
+      <c r="T28" s="3" t="s">
         <v>112</v>
       </c>
+      <c r="U28" s="3"/>
       <c r="V28" s="3"/>
       <c r="W28" s="3"/>
       <c r="X28" s="3"/>
@@ -3173,7 +3171,7 @@
       <c r="AE28" s="3"/>
       <c r="AF28" s="3"/>
     </row>
-    <row r="29" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>105</v>
       </c>
@@ -3191,30 +3189,30 @@
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
       <c r="I29" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J29" s="3"/>
-      <c r="K29" s="3"/>
+      <c r="K29" s="3" t="s">
+        <v>123</v>
+      </c>
       <c r="L29" s="3" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="M29" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="N29" s="3" t="s">
         <v>112</v>
       </c>
+      <c r="N29" s="3"/>
       <c r="O29" s="3"/>
       <c r="P29" s="3"/>
-      <c r="Q29" s="3"/>
-      <c r="R29" s="3" t="s">
-        <v>150</v>
-      </c>
+      <c r="Q29" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="R29" s="3"/>
       <c r="S29" s="3"/>
-      <c r="T29" s="3"/>
-      <c r="U29" s="3" t="s">
-        <v>138</v>
-      </c>
+      <c r="T29" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="U29" s="3"/>
       <c r="V29" s="3"/>
       <c r="W29" s="3"/>
       <c r="X29" s="3"/>
@@ -3227,7 +3225,7 @@
       <c r="AE29" s="3"/>
       <c r="AF29" s="3"/>
     </row>
-    <row r="30" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>105</v>
       </c>
@@ -3245,30 +3243,30 @@
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
       <c r="I30" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J30" s="3"/>
-      <c r="K30" s="3"/>
+      <c r="K30" s="3" t="s">
+        <v>123</v>
+      </c>
       <c r="L30" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="M30" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="N30" s="3" t="s">
         <v>111</v>
       </c>
+      <c r="N30" s="3"/>
       <c r="O30" s="3"/>
       <c r="P30" s="3"/>
-      <c r="Q30" s="3"/>
-      <c r="R30" s="3" t="s">
-        <v>148</v>
-      </c>
+      <c r="Q30" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="R30" s="3"/>
       <c r="S30" s="3"/>
-      <c r="T30" s="3"/>
-      <c r="U30" s="3" t="s">
-        <v>141</v>
-      </c>
+      <c r="T30" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="U30" s="3"/>
       <c r="V30" s="3"/>
       <c r="W30" s="3"/>
       <c r="X30" s="3"/>
@@ -3281,7 +3279,7 @@
       <c r="AE30" s="3"/>
       <c r="AF30" s="3"/>
     </row>
-    <row r="31" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>105</v>
       </c>
@@ -3299,30 +3297,30 @@
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
       <c r="I31" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J31" s="3"/>
-      <c r="K31" s="3"/>
+      <c r="K31" s="3" t="s">
+        <v>123</v>
+      </c>
       <c r="L31" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="M31" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="N31" s="3" t="s">
         <v>122</v>
       </c>
+      <c r="N31" s="3"/>
       <c r="O31" s="3"/>
       <c r="P31" s="3"/>
-      <c r="Q31" s="3"/>
-      <c r="R31" s="3" t="s">
-        <v>150</v>
-      </c>
+      <c r="Q31" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="R31" s="3"/>
       <c r="S31" s="3"/>
-      <c r="T31" s="3"/>
-      <c r="U31" s="3" t="s">
-        <v>142</v>
-      </c>
+      <c r="T31" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="U31" s="3"/>
       <c r="V31" s="3"/>
       <c r="W31" s="3"/>
       <c r="X31" s="3"/>
@@ -3335,7 +3333,7 @@
       <c r="AE31" s="3"/>
       <c r="AF31" s="3"/>
     </row>
-    <row r="32" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
         <v>105</v>
       </c>
@@ -3353,30 +3351,30 @@
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
       <c r="I32" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J32" s="3"/>
-      <c r="K32" s="3"/>
+      <c r="K32" s="3" t="s">
+        <v>123</v>
+      </c>
       <c r="L32" s="3" t="s">
-        <v>123</v>
+        <v>106</v>
       </c>
       <c r="M32" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="N32" s="3" t="s">
         <v>120</v>
       </c>
+      <c r="N32" s="3"/>
       <c r="O32" s="3"/>
       <c r="P32" s="3"/>
-      <c r="Q32" s="3"/>
-      <c r="R32" s="3" t="s">
-        <v>76</v>
-      </c>
+      <c r="Q32" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="R32" s="3"/>
       <c r="S32" s="3"/>
-      <c r="T32" s="3"/>
-      <c r="U32" s="3" t="s">
+      <c r="T32" s="3" t="s">
         <v>123</v>
       </c>
+      <c r="U32" s="3"/>
       <c r="V32" s="3"/>
       <c r="W32" s="3"/>
       <c r="X32" s="3"/>
@@ -3389,7 +3387,7 @@
       <c r="AE32" s="3"/>
       <c r="AF32" s="3"/>
     </row>
-    <row r="33" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
         <v>105</v>
       </c>
@@ -3407,34 +3405,32 @@
       <c r="G33" s="3"/>
       <c r="H33" s="3"/>
       <c r="I33" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="J33" s="3" t="s">
-        <v>126</v>
+        <v>108</v>
       </c>
       <c r="K33" s="3" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="L33" s="3" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="M33" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="N33" s="3" t="s">
         <v>112</v>
       </c>
+      <c r="N33" s="3"/>
       <c r="O33" s="3"/>
       <c r="P33" s="3"/>
-      <c r="Q33" s="3"/>
-      <c r="R33" s="3" t="s">
-        <v>76</v>
-      </c>
+      <c r="Q33" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="R33" s="3"/>
       <c r="S33" s="3"/>
-      <c r="T33" s="3"/>
-      <c r="U33" s="3" t="s">
-        <v>143</v>
-      </c>
+      <c r="T33" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="U33" s="3"/>
       <c r="V33" s="3"/>
       <c r="W33" s="3"/>
       <c r="X33" s="3"/>
@@ -3447,7 +3443,7 @@
       <c r="AE33" s="3"/>
       <c r="AF33" s="3"/>
     </row>
-    <row r="34" spans="1:32" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:32" ht="16" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="3">
         <v>1148</v>
       </c>
@@ -3455,16 +3451,16 @@
         <v>89</v>
       </c>
       <c r="C34" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="F34" s="3" t="s">
         <v>163</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="F34" s="3" t="s">
-        <v>164</v>
       </c>
       <c r="G34" s="3"/>
       <c r="H34" s="3"/>
@@ -3474,38 +3470,38 @@
       <c r="L34" s="3"/>
       <c r="M34" s="3"/>
       <c r="N34" s="3"/>
-      <c r="O34" s="3"/>
+      <c r="O34" s="3" t="s">
+        <v>138</v>
+      </c>
       <c r="P34" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="Q34" s="3" t="s">
-        <v>181</v>
-      </c>
+        <v>180</v>
+      </c>
+      <c r="Q34" s="3"/>
       <c r="R34" s="3"/>
-      <c r="S34" s="3"/>
-      <c r="T34" s="3" t="s">
-        <v>170</v>
-      </c>
+      <c r="S34" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="T34" s="3"/>
       <c r="U34" s="3"/>
-      <c r="V34" s="3"/>
-      <c r="W34" s="3" t="s">
+      <c r="V34" s="3" t="s">
         <v>89</v>
       </c>
+      <c r="W34" s="3"/>
       <c r="X34" s="3"/>
-      <c r="Y34" s="3"/>
-      <c r="Z34" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="AA34" s="3"/>
-      <c r="AB34" s="3" t="s">
-        <v>184</v>
-      </c>
+      <c r="Y34" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="Z34" s="3"/>
+      <c r="AA34" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="AB34" s="3"/>
       <c r="AC34" s="3"/>
       <c r="AD34" s="3"/>
       <c r="AE34" s="3"/>
       <c r="AF34" s="3"/>
     </row>
-    <row r="35" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A35" s="3">
         <v>1148</v>
       </c>
@@ -3513,16 +3509,16 @@
         <v>89</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>76</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G35" s="3"/>
       <c r="H35" s="3"/>
@@ -3532,38 +3528,38 @@
       <c r="L35" s="3"/>
       <c r="M35" s="3"/>
       <c r="N35" s="3"/>
-      <c r="O35" s="3"/>
+      <c r="O35" s="3" t="s">
+        <v>175</v>
+      </c>
       <c r="P35" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="Q35" s="3" t="s">
         <v>108</v>
       </c>
+      <c r="Q35" s="3"/>
       <c r="R35" s="3"/>
-      <c r="S35" s="3"/>
-      <c r="T35" s="3" t="s">
-        <v>171</v>
-      </c>
+      <c r="S35" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="T35" s="3"/>
       <c r="U35" s="3"/>
-      <c r="V35" s="3"/>
-      <c r="W35" s="3" t="s">
-        <v>76</v>
-      </c>
+      <c r="V35" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="W35" s="3"/>
       <c r="X35" s="3"/>
-      <c r="Y35" s="3"/>
-      <c r="Z35" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="AA35" s="3"/>
-      <c r="AB35" s="3" t="s">
-        <v>76</v>
-      </c>
+      <c r="Y35" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="Z35" s="3"/>
+      <c r="AA35" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="AB35" s="3"/>
       <c r="AC35" s="3"/>
       <c r="AD35" s="3"/>
       <c r="AE35" s="3"/>
       <c r="AF35" s="3"/>
     </row>
-    <row r="36" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A36" s="3">
         <v>1148</v>
       </c>
@@ -3571,14 +3567,14 @@
         <v>89</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E36" s="3"/>
       <c r="F36" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
@@ -3588,38 +3584,38 @@
       <c r="L36" s="3"/>
       <c r="M36" s="3"/>
       <c r="N36" s="3"/>
-      <c r="O36" s="3"/>
+      <c r="O36" s="3" t="s">
+        <v>175</v>
+      </c>
       <c r="P36" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="Q36" s="3" t="s">
         <v>108</v>
       </c>
+      <c r="Q36" s="3"/>
       <c r="R36" s="3"/>
-      <c r="S36" s="3"/>
-      <c r="T36" s="3" t="s">
-        <v>172</v>
-      </c>
+      <c r="S36" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="T36" s="3"/>
       <c r="U36" s="3"/>
-      <c r="V36" s="3"/>
-      <c r="W36" s="3" t="s">
+      <c r="V36" s="3" t="s">
         <v>92</v>
       </c>
+      <c r="W36" s="3"/>
       <c r="X36" s="3"/>
-      <c r="Y36" s="3"/>
-      <c r="Z36" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="AA36" s="3"/>
-      <c r="AB36" s="3" t="s">
-        <v>185</v>
-      </c>
+      <c r="Y36" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="Z36" s="3"/>
+      <c r="AA36" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="AB36" s="3"/>
       <c r="AC36" s="3"/>
       <c r="AD36" s="3"/>
       <c r="AE36" s="3"/>
       <c r="AF36" s="3"/>
     </row>
-    <row r="37" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A37" s="3">
         <v>1148</v>
       </c>
@@ -3627,10 +3623,10 @@
         <v>89</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E37" s="3"/>
       <c r="F37" s="3" t="s">
@@ -3644,38 +3640,38 @@
       <c r="L37" s="3"/>
       <c r="M37" s="3"/>
       <c r="N37" s="3"/>
-      <c r="O37" s="3"/>
+      <c r="O37" s="3" t="s">
+        <v>76</v>
+      </c>
       <c r="P37" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="Q37" s="3" t="s">
-        <v>76</v>
-      </c>
+      <c r="Q37" s="3"/>
       <c r="R37" s="3"/>
-      <c r="S37" s="3"/>
-      <c r="T37" s="3" t="s">
-        <v>173</v>
-      </c>
+      <c r="S37" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="T37" s="3"/>
       <c r="U37" s="3"/>
-      <c r="V37" s="3"/>
-      <c r="W37" s="3" t="s">
-        <v>170</v>
-      </c>
+      <c r="V37" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="W37" s="3"/>
       <c r="X37" s="3"/>
-      <c r="Y37" s="3"/>
-      <c r="Z37" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="AA37" s="3"/>
-      <c r="AB37" s="3" t="s">
+      <c r="Y37" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="Z37" s="3"/>
+      <c r="AA37" s="3" t="s">
         <v>86</v>
       </c>
+      <c r="AB37" s="3"/>
       <c r="AC37" s="3"/>
       <c r="AD37" s="3"/>
       <c r="AE37" s="3"/>
       <c r="AF37" s="3"/>
     </row>
-    <row r="38" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A38" s="3">
         <v>1148</v>
       </c>
@@ -3683,16 +3679,16 @@
         <v>89</v>
       </c>
       <c r="C38" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="F38" s="3" t="s">
         <v>163</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="F38" s="3" t="s">
-        <v>164</v>
       </c>
       <c r="G38" s="3"/>
       <c r="H38" s="3"/>
@@ -3702,38 +3698,38 @@
       <c r="L38" s="3"/>
       <c r="M38" s="3"/>
       <c r="N38" s="3"/>
-      <c r="O38" s="3"/>
+      <c r="O38" s="3" t="s">
+        <v>138</v>
+      </c>
       <c r="P38" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="Q38" s="3" t="s">
-        <v>181</v>
-      </c>
+        <v>180</v>
+      </c>
+      <c r="Q38" s="3"/>
       <c r="R38" s="3"/>
-      <c r="S38" s="3"/>
-      <c r="T38" s="3" t="s">
-        <v>174</v>
-      </c>
+      <c r="S38" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="T38" s="3"/>
       <c r="U38" s="3"/>
-      <c r="V38" s="3"/>
-      <c r="W38" s="3" t="s">
-        <v>189</v>
-      </c>
+      <c r="V38" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="W38" s="3"/>
       <c r="X38" s="3"/>
-      <c r="Y38" s="3"/>
-      <c r="Z38" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="AA38" s="3"/>
-      <c r="AB38" s="3" t="s">
-        <v>180</v>
-      </c>
+      <c r="Y38" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="Z38" s="3"/>
+      <c r="AA38" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="AB38" s="3"/>
       <c r="AC38" s="3"/>
       <c r="AD38" s="3"/>
       <c r="AE38" s="3"/>
       <c r="AF38" s="3"/>
     </row>
-    <row r="39" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A39" s="3">
         <v>1148</v>
       </c>
@@ -3741,16 +3737,16 @@
         <v>89</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G39" s="3"/>
       <c r="H39" s="3"/>
@@ -3760,40 +3756,40 @@
       <c r="L39" s="3"/>
       <c r="M39" s="3"/>
       <c r="N39" s="3"/>
-      <c r="O39" s="3"/>
+      <c r="O39" s="3" t="s">
+        <v>194</v>
+      </c>
       <c r="P39" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="Q39" s="3" t="s">
-        <v>197</v>
-      </c>
+        <v>196</v>
+      </c>
+      <c r="Q39" s="3"/>
       <c r="R39" s="3"/>
-      <c r="S39" s="3"/>
-      <c r="T39" s="3" t="s">
-        <v>175</v>
-      </c>
+      <c r="S39" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="T39" s="3"/>
       <c r="U39" s="3"/>
-      <c r="V39" s="3"/>
-      <c r="W39" s="3" t="s">
-        <v>136</v>
-      </c>
+      <c r="V39" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="W39" s="3"/>
       <c r="X39" s="3"/>
-      <c r="Y39" s="3"/>
-      <c r="Z39" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="AA39" s="3"/>
-      <c r="AB39" s="3" t="s">
-        <v>186</v>
-      </c>
+      <c r="Y39" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="Z39" s="3"/>
+      <c r="AA39" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="AB39" s="3"/>
       <c r="AC39" s="3"/>
       <c r="AD39" s="3"/>
       <c r="AE39" s="3"/>
       <c r="AF39" s="3" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="40" spans="1:32" x14ac:dyDescent="0.2">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="40" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A40" s="3">
         <v>1148</v>
       </c>
@@ -3801,16 +3797,16 @@
         <v>89</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G40" s="3"/>
       <c r="H40" s="3"/>
@@ -3820,40 +3816,40 @@
       <c r="L40" s="3"/>
       <c r="M40" s="3"/>
       <c r="N40" s="3"/>
-      <c r="O40" s="3"/>
+      <c r="O40" s="3" t="s">
+        <v>180</v>
+      </c>
       <c r="P40" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="Q40" s="3" t="s">
-        <v>181</v>
-      </c>
+        <v>180</v>
+      </c>
+      <c r="Q40" s="3"/>
       <c r="R40" s="3"/>
-      <c r="S40" s="3"/>
-      <c r="T40" s="3" t="s">
-        <v>176</v>
-      </c>
+      <c r="S40" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="T40" s="3"/>
       <c r="U40" s="3"/>
-      <c r="V40" s="3"/>
-      <c r="W40" s="3" t="s">
-        <v>193</v>
-      </c>
+      <c r="V40" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="W40" s="3"/>
       <c r="X40" s="3"/>
-      <c r="Y40" s="3"/>
-      <c r="Z40" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="AA40" s="3"/>
-      <c r="AB40" s="3" t="s">
-        <v>137</v>
-      </c>
+      <c r="Y40" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="Z40" s="3"/>
+      <c r="AA40" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="AB40" s="3"/>
       <c r="AC40" s="3"/>
       <c r="AD40" s="3"/>
       <c r="AE40" s="3"/>
       <c r="AF40" s="3" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="41" spans="1:32" x14ac:dyDescent="0.2">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="41" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A41" s="3">
         <v>1148</v>
       </c>
@@ -3861,16 +3857,16 @@
         <v>89</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G41" s="3"/>
       <c r="H41" s="3"/>
@@ -3880,40 +3876,40 @@
       <c r="L41" s="3"/>
       <c r="M41" s="3"/>
       <c r="N41" s="3"/>
-      <c r="O41" s="3"/>
+      <c r="O41" s="3" t="s">
+        <v>148</v>
+      </c>
       <c r="P41" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="Q41" s="3" t="s">
         <v>108</v>
       </c>
+      <c r="Q41" s="3"/>
       <c r="R41" s="3"/>
-      <c r="S41" s="3"/>
-      <c r="T41" s="3" t="s">
-        <v>177</v>
-      </c>
+      <c r="S41" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="T41" s="3"/>
       <c r="U41" s="3"/>
-      <c r="V41" s="3"/>
-      <c r="W41" s="3" t="s">
-        <v>189</v>
-      </c>
+      <c r="V41" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="W41" s="3"/>
       <c r="X41" s="3"/>
-      <c r="Y41" s="3"/>
-      <c r="Z41" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="AA41" s="3"/>
-      <c r="AB41" s="3" t="s">
-        <v>179</v>
-      </c>
+      <c r="Y41" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="Z41" s="3"/>
+      <c r="AA41" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="AB41" s="3"/>
       <c r="AC41" s="3"/>
       <c r="AD41" s="3"/>
       <c r="AE41" s="3"/>
       <c r="AF41" s="3" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="42" spans="1:32" x14ac:dyDescent="0.2">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="42" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A42" s="3">
         <v>1148</v>
       </c>
@@ -3921,14 +3917,14 @@
         <v>89</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E42" s="3"/>
       <c r="F42" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G42" s="3"/>
       <c r="H42" s="3"/>
@@ -3938,38 +3934,38 @@
       <c r="L42" s="3"/>
       <c r="M42" s="3"/>
       <c r="N42" s="3"/>
-      <c r="O42" s="3"/>
+      <c r="O42" s="3" t="s">
+        <v>76</v>
+      </c>
       <c r="P42" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q42" s="3" t="s">
-        <v>198</v>
-      </c>
+        <v>197</v>
+      </c>
+      <c r="Q42" s="3"/>
       <c r="R42" s="3"/>
-      <c r="S42" s="3"/>
-      <c r="T42" s="3" t="s">
-        <v>178</v>
-      </c>
+      <c r="S42" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="T42" s="3"/>
       <c r="U42" s="3"/>
-      <c r="V42" s="3"/>
-      <c r="W42" s="3" t="s">
-        <v>76</v>
-      </c>
+      <c r="V42" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="W42" s="3"/>
       <c r="X42" s="3"/>
-      <c r="Y42" s="3"/>
-      <c r="Z42" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="AA42" s="3"/>
-      <c r="AB42" s="3" t="s">
-        <v>76</v>
-      </c>
+      <c r="Y42" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="Z42" s="3"/>
+      <c r="AA42" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="AB42" s="3"/>
       <c r="AC42" s="3"/>
       <c r="AD42" s="3"/>
       <c r="AE42" s="3"/>
       <c r="AF42" s="3"/>
     </row>
-    <row r="43" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A43" s="3">
         <v>1148</v>
       </c>
@@ -3977,14 +3973,14 @@
         <v>89</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E43" s="3"/>
       <c r="F43" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G43" s="3"/>
       <c r="H43" s="3"/>
@@ -3994,38 +3990,38 @@
       <c r="L43" s="3"/>
       <c r="M43" s="3"/>
       <c r="N43" s="3"/>
-      <c r="O43" s="3"/>
+      <c r="O43" s="3" t="s">
+        <v>175</v>
+      </c>
       <c r="P43" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="Q43" s="3" t="s">
         <v>108</v>
       </c>
+      <c r="Q43" s="3"/>
       <c r="R43" s="3"/>
-      <c r="S43" s="3"/>
-      <c r="T43" s="3" t="s">
-        <v>172</v>
-      </c>
+      <c r="S43" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="T43" s="3"/>
       <c r="U43" s="3"/>
-      <c r="V43" s="3"/>
-      <c r="W43" s="3" t="s">
+      <c r="V43" s="3" t="s">
         <v>92</v>
       </c>
+      <c r="W43" s="3"/>
       <c r="X43" s="3"/>
-      <c r="Y43" s="3"/>
-      <c r="Z43" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="AA43" s="3"/>
-      <c r="AB43" s="3" t="s">
-        <v>187</v>
-      </c>
+      <c r="Y43" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="Z43" s="3"/>
+      <c r="AA43" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="AB43" s="3"/>
       <c r="AC43" s="3"/>
       <c r="AD43" s="3"/>
       <c r="AE43" s="3"/>
       <c r="AF43" s="3"/>
     </row>
-    <row r="44" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A44" s="3">
         <v>1148</v>
       </c>
@@ -4033,14 +4029,14 @@
         <v>89</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E44" s="3"/>
       <c r="F44" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G44" s="3"/>
       <c r="H44" s="3"/>
@@ -4050,38 +4046,38 @@
       <c r="L44" s="3"/>
       <c r="M44" s="3"/>
       <c r="N44" s="3"/>
-      <c r="O44" s="3"/>
+      <c r="O44" s="3" t="s">
+        <v>195</v>
+      </c>
       <c r="P44" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="Q44" s="3" t="s">
         <v>108</v>
       </c>
+      <c r="Q44" s="3"/>
       <c r="R44" s="3"/>
-      <c r="S44" s="3"/>
-      <c r="T44" s="3" t="s">
-        <v>176</v>
-      </c>
+      <c r="S44" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="T44" s="3"/>
       <c r="U44" s="3"/>
-      <c r="V44" s="3"/>
-      <c r="W44" s="3" t="s">
-        <v>138</v>
-      </c>
+      <c r="V44" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="W44" s="3"/>
       <c r="X44" s="3"/>
-      <c r="Y44" s="3"/>
-      <c r="Z44" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="AA44" s="3"/>
-      <c r="AB44" s="3" t="s">
-        <v>142</v>
-      </c>
+      <c r="Y44" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="Z44" s="3"/>
+      <c r="AA44" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="AB44" s="3"/>
       <c r="AC44" s="3"/>
       <c r="AD44" s="3"/>
       <c r="AE44" s="3"/>
       <c r="AF44" s="3"/>
     </row>
-    <row r="45" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A45" s="3">
         <v>1148</v>
       </c>
@@ -4089,14 +4085,14 @@
         <v>89</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E45" s="3"/>
       <c r="F45" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G45" s="3"/>
       <c r="H45" s="3"/>
@@ -4106,38 +4102,38 @@
       <c r="L45" s="3"/>
       <c r="M45" s="3"/>
       <c r="N45" s="3"/>
-      <c r="O45" s="3"/>
+      <c r="O45" s="3" t="s">
+        <v>175</v>
+      </c>
       <c r="P45" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="Q45" s="3" t="s">
         <v>108</v>
       </c>
+      <c r="Q45" s="3"/>
       <c r="R45" s="3"/>
-      <c r="S45" s="3"/>
-      <c r="T45" s="3" t="s">
+      <c r="S45" s="3" t="s">
         <v>111</v>
       </c>
+      <c r="T45" s="3"/>
       <c r="U45" s="3"/>
-      <c r="V45" s="3"/>
-      <c r="W45" s="3" t="s">
+      <c r="V45" s="3" t="s">
         <v>124</v>
       </c>
+      <c r="W45" s="3"/>
       <c r="X45" s="3"/>
-      <c r="Y45" s="3"/>
-      <c r="Z45" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="AA45" s="3"/>
-      <c r="AB45" s="3" t="s">
-        <v>188</v>
-      </c>
+      <c r="Y45" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="Z45" s="3"/>
+      <c r="AA45" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="AB45" s="3"/>
       <c r="AC45" s="3"/>
       <c r="AD45" s="3"/>
       <c r="AE45" s="3"/>
       <c r="AF45" s="3"/>
     </row>
-    <row r="46" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A46" s="3">
         <v>1148</v>
       </c>
@@ -4145,14 +4141,14 @@
         <v>89</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E46" s="3"/>
       <c r="F46" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G46" s="3"/>
       <c r="H46" s="3"/>
@@ -4162,38 +4158,38 @@
       <c r="L46" s="3"/>
       <c r="M46" s="3"/>
       <c r="N46" s="3"/>
-      <c r="O46" s="3"/>
+      <c r="O46" s="3" t="s">
+        <v>138</v>
+      </c>
       <c r="P46" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="Q46" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="Q46" s="3"/>
+      <c r="R46" s="3"/>
+      <c r="S46" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="T46" s="3"/>
+      <c r="U46" s="3"/>
+      <c r="V46" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="W46" s="3"/>
+      <c r="X46" s="3"/>
+      <c r="Y46" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="R46" s="3"/>
-      <c r="S46" s="3"/>
-      <c r="T46" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="U46" s="3"/>
-      <c r="V46" s="3"/>
-      <c r="W46" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="X46" s="3"/>
-      <c r="Y46" s="3"/>
-      <c r="Z46" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="AA46" s="3"/>
-      <c r="AB46" s="3" t="s">
-        <v>136</v>
-      </c>
+      <c r="Z46" s="3"/>
+      <c r="AA46" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="AB46" s="3"/>
       <c r="AC46" s="3"/>
       <c r="AD46" s="3"/>
       <c r="AE46" s="3"/>
       <c r="AF46" s="3"/>
     </row>
-    <row r="47" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A47" s="3">
         <v>1148</v>
       </c>
@@ -4201,14 +4197,14 @@
         <v>89</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E47" s="3"/>
       <c r="F47" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G47" s="3"/>
       <c r="H47" s="3"/>
@@ -4218,32 +4214,32 @@
       <c r="L47" s="3"/>
       <c r="M47" s="3"/>
       <c r="N47" s="3"/>
-      <c r="O47" s="3"/>
+      <c r="O47" s="3" t="s">
+        <v>175</v>
+      </c>
       <c r="P47" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="Q47" s="3" t="s">
         <v>108</v>
       </c>
+      <c r="Q47" s="3"/>
       <c r="R47" s="3"/>
-      <c r="S47" s="3"/>
-      <c r="T47" s="3" t="s">
-        <v>176</v>
-      </c>
+      <c r="S47" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="T47" s="3"/>
       <c r="U47" s="3"/>
-      <c r="V47" s="3"/>
-      <c r="W47" s="3" t="s">
-        <v>194</v>
-      </c>
+      <c r="V47" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="W47" s="3"/>
       <c r="X47" s="3"/>
-      <c r="Y47" s="3"/>
-      <c r="Z47" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="AA47" s="3"/>
-      <c r="AB47" s="3" t="s">
-        <v>187</v>
-      </c>
+      <c r="Y47" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="Z47" s="3"/>
+      <c r="AA47" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="AB47" s="3"/>
       <c r="AC47" s="3"/>
       <c r="AD47" s="3"/>
       <c r="AE47" s="3"/>

</xml_diff>

<commit_message>
just filtered out rows in table
</commit_message>
<xml_diff>
--- a/analyses/scrapeUSDAseedmanual/scraping/usdaDataScraping_CRD.xlsx
+++ b/analyses/scrapeUSDAseedmanual/scraping/usdaDataScraping_CRD.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10720"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PhD\Project\egret\analyses\scrapeUSDAseedmanual\scraping\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christophe_rouleau-desrochers/github/egret/analyses/scrapeUSDAseedmanual/scraping/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC624A39-11F7-4944-93CB-9A9997919DF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A7A6A28-D2BF-E34A-A33B-011154AEA2F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30" yWindow="5600" windowWidth="19270" windowHeight="5940" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="720" windowWidth="11980" windowHeight="18400" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Meta" sheetId="1" r:id="rId1"/>
@@ -717,13 +717,13 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -918,9 +918,9 @@
     <tableColumn id="26" xr3:uid="{5AE4612B-E138-4D40-8419-CC14A92B62CD}" name="germinative_capacity" dataDxfId="5"/>
     <tableColumn id="27" xr3:uid="{5BE09F3B-7D66-884A-B192-CEE49F2B845E}" name="percent_germination_15degC_incubated" dataDxfId="4"/>
     <tableColumn id="28" xr3:uid="{6061511F-2CE6-FF4C-BA21-079020EC6884}" name="percent_germination_20degC_incubated" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{89D5B3B5-8BC9-4BAA-8D45-AB924C4812E9}" name="germ_rate_days" dataDxfId="0"/>
-    <tableColumn id="29" xr3:uid="{B17A6158-E57A-8B49-B7C6-A792A8BB3857}" name="50%_germ" dataDxfId="2"/>
-    <tableColumn id="30" xr3:uid="{C6852079-746D-E843-96F0-451DDB3F34C3}" name="Notes" dataDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{89D5B3B5-8BC9-4BAA-8D45-AB924C4812E9}" name="germ_rate_days" dataDxfId="2"/>
+    <tableColumn id="29" xr3:uid="{B17A6158-E57A-8B49-B7C6-A792A8BB3857}" name="50%_germ" dataDxfId="1"/>
+    <tableColumn id="30" xr3:uid="{C6852079-746D-E843-96F0-451DDB3F34C3}" name="Notes" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1195,7 +1195,7 @@
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="41.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
@@ -1209,7 +1209,7 @@
     <col min="10" max="10" width="41.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1251,7 +1251,7 @@
       <c r="AI1" s="1"/>
       <c r="AJ1" s="1"/>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1259,7 +1259,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1267,7 +1267,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -1275,7 +1275,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1283,7 +1283,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1291,7 +1291,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -1299,7 +1299,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -1307,7 +1307,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -1315,7 +1315,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -1323,7 +1323,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -1331,7 +1331,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -1339,7 +1339,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -1347,7 +1347,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
@@ -1355,7 +1355,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -1363,7 +1363,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -1371,7 +1371,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
@@ -1379,7 +1379,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>66</v>
       </c>
@@ -1387,7 +1387,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>65</v>
       </c>
@@ -1395,7 +1395,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>64</v>
       </c>
@@ -1403,7 +1403,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
@@ -1411,7 +1411,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
@@ -1419,7 +1419,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
@@ -1427,7 +1427,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
@@ -1435,7 +1435,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
@@ -1443,7 +1443,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
@@ -1451,7 +1451,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>26</v>
       </c>
@@ -1459,7 +1459,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>27</v>
       </c>
@@ -1467,7 +1467,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>52</v>
       </c>
@@ -1475,7 +1475,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>53</v>
       </c>
@@ -1483,22 +1483,22 @@
         <v>58</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>63</v>
       </c>
@@ -1514,11 +1514,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4AC4DDB-17EE-463A-9304-F699F6DBC2E2}">
   <dimension ref="A1:AF47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AB1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="AG2" sqref="AG2"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.83203125" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
@@ -1549,7 +1549,7 @@
     <col min="32" max="32" width="8.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1647,7 +1647,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>703</v>
       </c>
@@ -1707,7 +1707,7 @@
       <c r="AE2" s="3"/>
       <c r="AF2" s="3"/>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>703</v>
       </c>
@@ -1767,7 +1767,7 @@
       <c r="AE3" s="3"/>
       <c r="AF3" s="3"/>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>703</v>
       </c>
@@ -1827,7 +1827,7 @@
       <c r="AE4" s="3"/>
       <c r="AF4" s="3"/>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>703</v>
       </c>
@@ -1887,7 +1887,7 @@
       <c r="AE5" s="3"/>
       <c r="AF5" s="3"/>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>703</v>
       </c>
@@ -1947,7 +1947,7 @@
       <c r="AE6" s="3"/>
       <c r="AF6" s="3"/>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>703</v>
       </c>
@@ -2013,7 +2013,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>703</v>
       </c>
@@ -2073,7 +2073,7 @@
       <c r="AE8" s="3"/>
       <c r="AF8" s="3"/>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>105</v>
       </c>
@@ -2129,7 +2129,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>105</v>
       </c>
@@ -2187,7 +2187,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>105</v>
       </c>
@@ -2243,7 +2243,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>105</v>
       </c>
@@ -2299,7 +2299,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>105</v>
       </c>
@@ -2353,7 +2353,7 @@
       <c r="AE13" s="3"/>
       <c r="AF13" s="3"/>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>105</v>
       </c>
@@ -2409,7 +2409,7 @@
       <c r="AE14" s="3"/>
       <c r="AF14" s="3"/>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>105</v>
       </c>
@@ -2465,7 +2465,7 @@
       <c r="AE15" s="3"/>
       <c r="AF15" s="3"/>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>105</v>
       </c>
@@ -2519,7 +2519,7 @@
       <c r="AE16" s="3"/>
       <c r="AF16" s="3"/>
     </row>
-    <row r="17" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>105</v>
       </c>
@@ -2573,7 +2573,7 @@
       <c r="AE17" s="3"/>
       <c r="AF17" s="3"/>
     </row>
-    <row r="18" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>105</v>
       </c>
@@ -2627,7 +2627,7 @@
       <c r="AE18" s="3"/>
       <c r="AF18" s="3"/>
     </row>
-    <row r="19" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>105</v>
       </c>
@@ -2681,7 +2681,7 @@
       <c r="AE19" s="3"/>
       <c r="AF19" s="3"/>
     </row>
-    <row r="20" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>105</v>
       </c>
@@ -2735,7 +2735,7 @@
       <c r="AE20" s="3"/>
       <c r="AF20" s="3"/>
     </row>
-    <row r="21" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>105</v>
       </c>
@@ -2789,7 +2789,7 @@
       <c r="AE21" s="3"/>
       <c r="AF21" s="3"/>
     </row>
-    <row r="22" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>105</v>
       </c>
@@ -2843,7 +2843,7 @@
       <c r="AE22" s="3"/>
       <c r="AF22" s="3"/>
     </row>
-    <row r="23" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>105</v>
       </c>
@@ -2897,7 +2897,7 @@
       <c r="AE23" s="3"/>
       <c r="AF23" s="3"/>
     </row>
-    <row r="24" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>105</v>
       </c>
@@ -2953,7 +2953,7 @@
       <c r="AE24" s="3"/>
       <c r="AF24" s="3"/>
     </row>
-    <row r="25" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>105</v>
       </c>
@@ -3007,7 +3007,7 @@
       <c r="AE25" s="3"/>
       <c r="AF25" s="3"/>
     </row>
-    <row r="26" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>105</v>
       </c>
@@ -3063,7 +3063,7 @@
       <c r="AE26" s="3"/>
       <c r="AF26" s="3"/>
     </row>
-    <row r="27" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>105</v>
       </c>
@@ -3117,7 +3117,7 @@
       <c r="AE27" s="3"/>
       <c r="AF27" s="3"/>
     </row>
-    <row r="28" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>105</v>
       </c>
@@ -3171,7 +3171,7 @@
       <c r="AE28" s="3"/>
       <c r="AF28" s="3"/>
     </row>
-    <row r="29" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>105</v>
       </c>
@@ -3225,7 +3225,7 @@
       <c r="AE29" s="3"/>
       <c r="AF29" s="3"/>
     </row>
-    <row r="30" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>105</v>
       </c>
@@ -3279,7 +3279,7 @@
       <c r="AE30" s="3"/>
       <c r="AF30" s="3"/>
     </row>
-    <row r="31" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>105</v>
       </c>
@@ -3333,7 +3333,7 @@
       <c r="AE31" s="3"/>
       <c r="AF31" s="3"/>
     </row>
-    <row r="32" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>105</v>
       </c>
@@ -3387,7 +3387,7 @@
       <c r="AE32" s="3"/>
       <c r="AF32" s="3"/>
     </row>
-    <row r="33" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>105</v>
       </c>
@@ -3443,7 +3443,7 @@
       <c r="AE33" s="3"/>
       <c r="AF33" s="3"/>
     </row>
-    <row r="34" spans="1:32" ht="16" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:32" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="3">
         <v>1148</v>
       </c>
@@ -3501,7 +3501,7 @@
       <c r="AE34" s="3"/>
       <c r="AF34" s="3"/>
     </row>
-    <row r="35" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A35" s="3">
         <v>1148</v>
       </c>
@@ -3559,7 +3559,7 @@
       <c r="AE35" s="3"/>
       <c r="AF35" s="3"/>
     </row>
-    <row r="36" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A36" s="3">
         <v>1148</v>
       </c>
@@ -3615,7 +3615,7 @@
       <c r="AE36" s="3"/>
       <c r="AF36" s="3"/>
     </row>
-    <row r="37" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A37" s="3">
         <v>1148</v>
       </c>
@@ -3671,7 +3671,7 @@
       <c r="AE37" s="3"/>
       <c r="AF37" s="3"/>
     </row>
-    <row r="38" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A38" s="3">
         <v>1148</v>
       </c>
@@ -3729,7 +3729,7 @@
       <c r="AE38" s="3"/>
       <c r="AF38" s="3"/>
     </row>
-    <row r="39" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A39" s="3">
         <v>1148</v>
       </c>
@@ -3789,7 +3789,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="40" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A40" s="3">
         <v>1148</v>
       </c>
@@ -3849,7 +3849,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="41" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A41" s="3">
         <v>1148</v>
       </c>
@@ -3909,7 +3909,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="42" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A42" s="3">
         <v>1148</v>
       </c>
@@ -3965,7 +3965,7 @@
       <c r="AE42" s="3"/>
       <c r="AF42" s="3"/>
     </row>
-    <row r="43" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A43" s="3">
         <v>1148</v>
       </c>
@@ -4021,7 +4021,7 @@
       <c r="AE43" s="3"/>
       <c r="AF43" s="3"/>
     </row>
-    <row r="44" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A44" s="3">
         <v>1148</v>
       </c>
@@ -4077,7 +4077,7 @@
       <c r="AE44" s="3"/>
       <c r="AF44" s="3"/>
     </row>
-    <row r="45" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A45" s="3">
         <v>1148</v>
       </c>
@@ -4133,7 +4133,7 @@
       <c r="AE45" s="3"/>
       <c r="AF45" s="3"/>
     </row>
-    <row r="46" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A46" s="3">
         <v>1148</v>
       </c>
@@ -4189,7 +4189,7 @@
       <c r="AE46" s="3"/>
       <c r="AF46" s="3"/>
     </row>
-    <row r="47" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A47" s="3">
         <v>1148</v>
       </c>

</xml_diff>